<commit_message>
completed open / close round UI functionality and debugged bootstrap bid.csv and the min bid error (e$<10 bids) as well as updated testcases
Co-Authored-By: hilyamy2018 <hilyamy2018@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mygit\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704C1F7B-C326-4C81-A8BF-8580DA540A26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA2AC23-11A7-4A31-9216-04B5BC3A9FA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -616,6 +616,9 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -665,9 +668,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,16 +1218,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
@@ -1274,11 +1274,11 @@
       <c r="F3" s="26">
         <v>5</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="49">
         <f>SUM(F3:F10)</f>
         <v>41</v>
       </c>
-      <c r="H3" s="39" t="str">
+      <c r="H3" s="40" t="str">
         <f xml:space="preserve"> IF(G3&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1302,8 +1302,8 @@
       <c r="F4" s="26">
         <v>1</v>
       </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="40"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26">
@@ -1324,8 +1324,8 @@
       <c r="F5" s="26">
         <v>5</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="40"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26">
@@ -1346,8 +1346,8 @@
       <c r="F6" s="26">
         <v>5</v>
       </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="40"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26">
@@ -1368,8 +1368,8 @@
       <c r="F7" s="26">
         <v>10</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="41"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="26">
@@ -1390,8 +1390,8 @@
       <c r="F8" s="26">
         <v>5</v>
       </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="42" t="s">
+      <c r="G8" s="50"/>
+      <c r="H8" s="43" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1414,8 +1414,8 @@
       <c r="F9" s="26">
         <v>5</v>
       </c>
-      <c r="G9" s="49"/>
-      <c r="H9" s="43"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="26">
@@ -1436,8 +1436,8 @@
       <c r="F10" s="26">
         <v>5</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="44"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="45"/>
     </row>
     <row r="11" spans="1:8" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
@@ -1515,7 +1515,7 @@
       <c r="G13" s="35">
         <v>10</v>
       </c>
-      <c r="H13" s="39" t="str">
+      <c r="H13" s="40" t="str">
         <f xml:space="preserve"> IF(G13:G14&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1542,7 +1542,7 @@
       <c r="G14" s="36">
         <v>10</v>
       </c>
-      <c r="H14" s="41"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15" spans="1:8" ht="43.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26">
@@ -1590,11 +1590,11 @@
       <c r="F16" s="26">
         <v>5</v>
       </c>
-      <c r="G16" s="49">
+      <c r="G16" s="50">
         <f>SUM(F16:F18)</f>
         <v>11</v>
       </c>
-      <c r="H16" s="46" t="str">
+      <c r="H16" s="47" t="str">
         <f xml:space="preserve"> IF(G16&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1618,8 +1618,8 @@
       <c r="F17" s="26">
         <v>1</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="47"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="48"/>
     </row>
     <row r="18" spans="1:8" ht="15.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
@@ -1640,8 +1640,8 @@
       <c r="F18" s="26">
         <v>5</v>
       </c>
-      <c r="G18" s="49"/>
-      <c r="H18" s="51"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="52"/>
     </row>
     <row r="19" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33">
@@ -1662,11 +1662,11 @@
       <c r="F19" s="26">
         <v>1</v>
       </c>
-      <c r="G19" s="52">
+      <c r="G19" s="53">
         <f>11</f>
         <v>11</v>
       </c>
-      <c r="H19" s="46" t="str">
+      <c r="H19" s="47" t="str">
         <f xml:space="preserve"> IF(G19&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1691,8 +1691,8 @@
         <f t="shared" ref="F20:F181" si="0">IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="51"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="52"/>
     </row>
     <row r="21" spans="1:8" ht="44" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
@@ -1854,10 +1854,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G26" s="45">
+      <c r="G26" s="46">
         <v>10</v>
       </c>
-      <c r="H26" s="46" t="str">
+      <c r="H26" s="47" t="str">
         <f xml:space="preserve"> IF(G26&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1882,8 +1882,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G27" s="45"/>
-      <c r="H27" s="47"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="48"/>
     </row>
     <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="19">
@@ -1892,7 +1892,7 @@
       <c r="B28" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="38" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="10" t="s">
@@ -6975,16 +6975,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
debugged authenticate.php, added function to do common json validations in common.php, updated bm
Co-Authored-By: j1em1n <j1em1n@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\GitHub\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B355C8E5-1BEE-4ED7-B3E5-6E364C95459F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B9F729-ECAF-4404-AE1A-CCA03C56E769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -639,6 +639,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1172,7 +1175,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="72" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1957,7 @@
       <c r="G32" s="49"/>
       <c r="H32" s="35"/>
     </row>
-    <row r="33" spans="1:6" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>31</v>
       </c>
@@ -1974,8 +1977,16 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="52">
+        <f>SUM(F33:F34)</f>
+        <v>6</v>
+      </c>
+      <c r="H33" s="35" t="str">
+        <f xml:space="preserve"> IF(G33&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>32</v>
       </c>
@@ -1995,8 +2006,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="G34" s="52"/>
+      <c r="H34" s="35"/>
+    </row>
+    <row r="35" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>33</v>
       </c>
@@ -2006,8 +2019,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H35" s="20" t="str">
+        <f xml:space="preserve"> IF(G35&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>34</v>
       </c>
@@ -2017,8 +2034,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H36" s="20" t="str">
+        <f xml:space="preserve"> IF(G36&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>35</v>
       </c>
@@ -2028,8 +2049,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H37" s="20" t="str">
+        <f xml:space="preserve"> IF(G37&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>36</v>
       </c>
@@ -2039,8 +2064,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H38" s="20" t="str">
+        <f xml:space="preserve"> IF(G38&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>37</v>
       </c>
@@ -2050,8 +2079,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H39" s="20" t="str">
+        <f xml:space="preserve"> IF(G39&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>38</v>
       </c>
@@ -2061,8 +2094,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H40" s="20" t="str">
+        <f xml:space="preserve"> IF(G40&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>39</v>
       </c>
@@ -2072,8 +2109,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H41" s="20" t="str">
+        <f xml:space="preserve"> IF(G41&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>40</v>
       </c>
@@ -2083,8 +2124,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H42" s="20" t="str">
+        <f xml:space="preserve"> IF(G42&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>41</v>
       </c>
@@ -2094,8 +2139,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H43" s="20" t="str">
+        <f xml:space="preserve"> IF(G43&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A44" s="19">
         <v>42</v>
       </c>
@@ -2105,8 +2154,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H44" s="20" t="str">
+        <f xml:space="preserve"> IF(G44&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
         <v>43</v>
       </c>
@@ -2116,8 +2169,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H45" s="20" t="str">
+        <f xml:space="preserve"> IF(G45&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A46" s="19">
         <v>44</v>
       </c>
@@ -2127,8 +2184,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H46" s="20" t="str">
+        <f xml:space="preserve"> IF(G46&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
         <v>45</v>
       </c>
@@ -2138,8 +2199,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H47" s="20" t="str">
+        <f xml:space="preserve"> IF(G47&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
         <v>46</v>
       </c>
@@ -2149,8 +2214,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H48" s="20" t="str">
+        <f xml:space="preserve"> IF(G48&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
         <v>47</v>
       </c>
@@ -2160,8 +2229,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H49" s="20" t="str">
+        <f xml:space="preserve"> IF(G49&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A50" s="19">
         <v>48</v>
       </c>
@@ -2171,8 +2244,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H50" s="20" t="str">
+        <f xml:space="preserve"> IF(G50&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A51" s="19">
         <v>49</v>
       </c>
@@ -2182,8 +2259,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H51" s="20" t="str">
+        <f xml:space="preserve"> IF(G51&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A52" s="19">
         <v>50</v>
       </c>
@@ -2193,8 +2274,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H52" s="20" t="str">
+        <f xml:space="preserve"> IF(G52&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
         <v>51</v>
       </c>
@@ -2204,8 +2289,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H53" s="20" t="str">
+        <f xml:space="preserve"> IF(G53&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
         <v>52</v>
       </c>
@@ -2215,8 +2304,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H54" s="20" t="str">
+        <f xml:space="preserve"> IF(G54&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
         <v>53</v>
       </c>
@@ -2226,8 +2319,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H55" s="20" t="str">
+        <f xml:space="preserve"> IF(G55&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A56" s="19">
         <v>54</v>
       </c>
@@ -2237,8 +2334,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H56" s="20" t="str">
+        <f xml:space="preserve"> IF(G56&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
         <v>55</v>
       </c>
@@ -2248,8 +2349,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H57" s="20" t="str">
+        <f xml:space="preserve"> IF(G57&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A58" s="19">
         <v>56</v>
       </c>
@@ -2259,8 +2364,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H58" s="20" t="str">
+        <f xml:space="preserve"> IF(G58&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A59" s="19">
         <v>57</v>
       </c>
@@ -2270,8 +2379,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H59" s="20" t="str">
+        <f xml:space="preserve"> IF(G59&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A60" s="19">
         <v>58</v>
       </c>
@@ -2281,8 +2394,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H60" s="20" t="str">
+        <f xml:space="preserve"> IF(G60&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A61" s="19">
         <v>59</v>
       </c>
@@ -2292,8 +2409,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H61" s="20" t="str">
+        <f xml:space="preserve"> IF(G61&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A62" s="19">
         <v>60</v>
       </c>
@@ -2303,8 +2424,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H62" s="20" t="str">
+        <f xml:space="preserve"> IF(G62&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A63" s="19">
         <v>61</v>
       </c>
@@ -2314,8 +2439,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
+      <c r="H63" s="20" t="str">
+        <f xml:space="preserve"> IF(G63&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A64" s="19">
         <v>62</v>
       </c>
@@ -2325,6 +2454,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="H64" s="20" t="str">
+        <f xml:space="preserve"> IF(G64&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="14.6" x14ac:dyDescent="0.25">
       <c r="A65" s="19">
@@ -6909,7 +7042,9 @@
       <c r="A1000" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
     <mergeCell ref="H28:H32"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="H3:H7"/>
@@ -6923,7 +7058,7 @@
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="G20:G32"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H2 H28 H33:H1048576">
+  <conditionalFormatting sqref="H1:H2 H28 H33 H35:H1048576">
     <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
@@ -6943,7 +7078,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
conducted Iter4 testing (uat-manual + json)
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\GitHub\project-g1t8\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FB8BEF-4B51-4D9C-80D5-B86DE32F816B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1807CD6B-29A7-4D47-B4BA-171CE02A5378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="177">
   <si>
     <t>Bug Log</t>
   </si>
@@ -1414,10 +1414,10 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" customWidth="1"/>
-    <col min="2" max="2" width="84.36328125" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="84.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1490,20 +1490,20 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" zoomScale="72" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+      <selection activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="74.54296875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="6.36328125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" style="35" customWidth="1"/>
-    <col min="8" max="8" width="34.54296875" style="33" customWidth="1"/>
-    <col min="9" max="16384" width="14.453125" style="19"/>
+    <col min="1" max="1" width="10.6640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="74.5546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="35" customWidth="1"/>
+    <col min="8" max="8" width="34.5546875" style="33" customWidth="1"/>
+    <col min="9" max="16384" width="14.44140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
       <c r="G1" s="41"/>
       <c r="H1" s="41"/>
     </row>
-    <row r="2" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
         <v>1</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <v>2</v>
       </c>
@@ -1594,7 +1594,7 @@
       <c r="G4" s="46"/>
       <c r="H4" s="43"/>
     </row>
-    <row r="5" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
         <v>3</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="G5" s="46"/>
       <c r="H5" s="43"/>
     </row>
-    <row r="6" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <v>4</v>
       </c>
@@ -1638,7 +1638,7 @@
       <c r="G6" s="46"/>
       <c r="H6" s="43"/>
     </row>
-    <row r="7" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
         <v>5</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="G7" s="46"/>
       <c r="H7" s="44"/>
     </row>
-    <row r="8" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25">
         <v>6</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25">
         <v>7</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25">
         <v>8</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
     </row>
-    <row r="11" spans="1:8" ht="44.35" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25">
         <v>9</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25">
         <v>10</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
         <v>11</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25">
         <v>12</v>
       </c>
@@ -1828,7 +1828,7 @@
       <c r="G14" s="46"/>
       <c r="H14" s="44"/>
     </row>
-    <row r="15" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25">
         <v>13</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>14</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30">
         <v>15</v>
       </c>
@@ -1900,7 +1900,7 @@
       <c r="G17" s="46"/>
       <c r="H17" s="43"/>
     </row>
-    <row r="18" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30">
         <v>16</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="H18" s="44"/>
     </row>
-    <row r="19" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="31">
         <v>17</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>18</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="H20" s="44"/>
     </row>
-    <row r="21" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>19</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
         <v>20</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>21</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>22</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18">
         <v>23</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>24</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18">
         <v>25</v>
       </c>
@@ -2154,7 +2154,7 @@
       <c r="G27" s="48"/>
       <c r="H27" s="43"/>
     </row>
-    <row r="28" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18">
         <v>26</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18">
         <v>27</v>
       </c>
@@ -2203,7 +2203,7 @@
       <c r="G29" s="48"/>
       <c r="H29" s="40"/>
     </row>
-    <row r="30" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18">
         <v>28</v>
       </c>
@@ -2226,7 +2226,7 @@
       <c r="G30" s="48"/>
       <c r="H30" s="40"/>
     </row>
-    <row r="31" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>29</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="G31" s="48"/>
       <c r="H31" s="40"/>
     </row>
-    <row r="32" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18">
         <v>30</v>
       </c>
@@ -2272,7 +2272,7 @@
       <c r="G32" s="48"/>
       <c r="H32" s="40"/>
     </row>
-    <row r="33" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
         <v>31</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18">
         <v>32</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="G34" s="39"/>
       <c r="H34" s="40"/>
     </row>
-    <row r="35" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
         <v>33</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="G38" s="39"/>
       <c r="H38" s="40"/>
     </row>
-    <row r="39" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18">
         <v>37</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="G39" s="39"/>
       <c r="H39" s="40"/>
     </row>
-    <row r="40" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
         <v>38</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="G40" s="39"/>
       <c r="H40" s="40"/>
     </row>
-    <row r="41" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18">
         <v>39</v>
       </c>
@@ -2485,7 +2485,7 @@
       <c r="G41" s="39"/>
       <c r="H41" s="40"/>
     </row>
-    <row r="42" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
         <v>40</v>
       </c>
@@ -2508,7 +2508,7 @@
       <c r="G42" s="39"/>
       <c r="H42" s="40"/>
     </row>
-    <row r="43" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
         <v>41</v>
       </c>
@@ -2531,7 +2531,7 @@
       <c r="G43" s="39"/>
       <c r="H43" s="40"/>
     </row>
-    <row r="44" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18">
         <v>42</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="G44" s="39"/>
       <c r="H44" s="40"/>
     </row>
-    <row r="45" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18">
         <v>43</v>
       </c>
@@ -2577,7 +2577,7 @@
       <c r="G45" s="39"/>
       <c r="H45" s="40"/>
     </row>
-    <row r="46" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18">
         <v>44</v>
       </c>
@@ -2600,7 +2600,7 @@
       <c r="G46" s="39"/>
       <c r="H46" s="40"/>
     </row>
-    <row r="47" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
         <v>45</v>
       </c>
@@ -2623,7 +2623,7 @@
       <c r="G47" s="39"/>
       <c r="H47" s="40"/>
     </row>
-    <row r="48" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
         <v>46</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="G48" s="39"/>
       <c r="H48" s="40"/>
     </row>
-    <row r="49" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
         <v>47</v>
       </c>
@@ -2669,7 +2669,7 @@
       <c r="G49" s="39"/>
       <c r="H49" s="40"/>
     </row>
-    <row r="50" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
         <v>48</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="G50" s="39"/>
       <c r="H50" s="40"/>
     </row>
-    <row r="51" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
         <v>49</v>
       </c>
@@ -2715,7 +2715,7 @@
       <c r="G51" s="39"/>
       <c r="H51" s="40"/>
     </row>
-    <row r="52" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
         <v>50</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="G52" s="39"/>
       <c r="H52" s="40"/>
     </row>
-    <row r="53" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
         <v>51</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="G53" s="39"/>
       <c r="H53" s="40"/>
     </row>
-    <row r="54" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18">
         <v>52</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="29.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18">
         <v>53</v>
       </c>
@@ -2836,7 +2836,7 @@
       <c r="G56" s="39"/>
       <c r="H56" s="40"/>
     </row>
-    <row r="57" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
         <v>55</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="G57" s="39"/>
       <c r="H57" s="40"/>
     </row>
-    <row r="58" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
         <v>56</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="G58" s="39"/>
       <c r="H58" s="40"/>
     </row>
-    <row r="59" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
         <v>57</v>
       </c>
@@ -2905,7 +2905,7 @@
       <c r="G59" s="39"/>
       <c r="H59" s="40"/>
     </row>
-    <row r="60" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
         <v>58</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="G60" s="39"/>
       <c r="H60" s="40"/>
     </row>
-    <row r="61" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <v>59</v>
       </c>
@@ -2951,7 +2951,7 @@
       <c r="G61" s="39"/>
       <c r="H61" s="40"/>
     </row>
-    <row r="62" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
         <v>60</v>
       </c>
@@ -2974,7 +2974,7 @@
       <c r="G62" s="39"/>
       <c r="H62" s="40"/>
     </row>
-    <row r="63" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
         <v>61</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="G63" s="39"/>
       <c r="H63" s="40"/>
     </row>
-    <row r="64" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
         <v>62</v>
       </c>
@@ -3020,7 +3020,7 @@
       <c r="G64" s="39"/>
       <c r="H64" s="40"/>
     </row>
-    <row r="65" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18">
         <v>63</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="G66" s="39"/>
       <c r="H66" s="40"/>
     </row>
-    <row r="67" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A67" s="36">
         <v>65</v>
       </c>
@@ -3158,7 +3158,7 @@
       <c r="G70" s="39"/>
       <c r="H70" s="40"/>
     </row>
-    <row r="71" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A71" s="36">
         <v>69</v>
       </c>
@@ -3181,7 +3181,7 @@
       <c r="G71" s="39"/>
       <c r="H71" s="40"/>
     </row>
-    <row r="72" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A72" s="36">
         <v>70</v>
       </c>
@@ -3204,7 +3204,7 @@
       <c r="G72" s="39"/>
       <c r="H72" s="40"/>
     </row>
-    <row r="73" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A73" s="36">
         <v>71</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="G73" s="39"/>
       <c r="H73" s="40"/>
     </row>
-    <row r="74" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A74" s="36">
         <v>72</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="G75" s="39"/>
       <c r="H75" s="40"/>
     </row>
-    <row r="76" spans="1:8" ht="43.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A76" s="36">
         <v>74</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="G78" s="39"/>
       <c r="H78" s="40"/>
     </row>
-    <row r="79" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A79" s="36">
         <v>77</v>
       </c>
@@ -3365,7 +3365,7 @@
       <c r="G79" s="39"/>
       <c r="H79" s="40"/>
     </row>
-    <row r="80" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A80" s="36">
         <v>78</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="G80" s="39"/>
       <c r="H80" s="40"/>
     </row>
-    <row r="81" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A81" s="36">
         <v>79</v>
       </c>
@@ -3503,7 +3503,7 @@
       <c r="G85" s="39"/>
       <c r="H85" s="40"/>
     </row>
-    <row r="86" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A86" s="36">
         <v>84</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="G87" s="39"/>
       <c r="H87" s="40"/>
     </row>
-    <row r="88" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A88" s="36">
         <v>86</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="G95" s="39"/>
       <c r="H95" s="40"/>
     </row>
-    <row r="96" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A96" s="36">
         <v>94</v>
       </c>
@@ -3756,7 +3756,7 @@
       <c r="G96" s="39"/>
       <c r="H96" s="40"/>
     </row>
-    <row r="97" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A97" s="36">
         <v>95</v>
       </c>
@@ -3779,7 +3779,7 @@
       <c r="G97" s="39"/>
       <c r="H97" s="40"/>
     </row>
-    <row r="98" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A98" s="36">
         <v>96</v>
       </c>
@@ -3802,7 +3802,7 @@
       <c r="G98" s="39"/>
       <c r="H98" s="40"/>
     </row>
-    <row r="99" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A99" s="36">
         <v>97</v>
       </c>
@@ -3825,7 +3825,7 @@
       <c r="G99" s="39"/>
       <c r="H99" s="40"/>
     </row>
-    <row r="100" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A100" s="36">
         <v>98</v>
       </c>
@@ -3871,7 +3871,7 @@
       <c r="G101" s="39"/>
       <c r="H101" s="40"/>
     </row>
-    <row r="102" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A102" s="36">
         <v>100</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="G106" s="39"/>
       <c r="H106" s="40"/>
     </row>
-    <row r="107" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A107" s="36">
         <v>105</v>
       </c>
@@ -4009,7 +4009,7 @@
       <c r="G107" s="39"/>
       <c r="H107" s="40"/>
     </row>
-    <row r="108" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A108" s="36">
         <v>106</v>
       </c>
@@ -4032,7 +4032,7 @@
       <c r="G108" s="39"/>
       <c r="H108" s="40"/>
     </row>
-    <row r="109" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A109" s="36">
         <v>107</v>
       </c>
@@ -4055,7 +4055,7 @@
       <c r="G109" s="39"/>
       <c r="H109" s="40"/>
     </row>
-    <row r="110" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A110" s="36">
         <v>108</v>
       </c>
@@ -4124,7 +4124,7 @@
       <c r="G112" s="39"/>
       <c r="H112" s="40"/>
     </row>
-    <row r="113" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A113" s="36">
         <v>111</v>
       </c>
@@ -4147,7 +4147,7 @@
       <c r="G113" s="39"/>
       <c r="H113" s="40"/>
     </row>
-    <row r="114" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A114" s="36">
         <v>112</v>
       </c>
@@ -4193,7 +4193,7 @@
       <c r="G115" s="39"/>
       <c r="H115" s="40"/>
     </row>
-    <row r="116" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A116" s="36">
         <v>114</v>
       </c>
@@ -4216,7 +4216,7 @@
       <c r="G116" s="39"/>
       <c r="H116" s="40"/>
     </row>
-    <row r="117" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A117" s="36">
         <v>115</v>
       </c>
@@ -4239,7 +4239,7 @@
       <c r="G117" s="39"/>
       <c r="H117" s="40"/>
     </row>
-    <row r="118" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A118" s="36">
         <v>116</v>
       </c>
@@ -4262,7 +4262,7 @@
       <c r="G118" s="39"/>
       <c r="H118" s="40"/>
     </row>
-    <row r="119" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A119" s="36">
         <v>117</v>
       </c>
@@ -4285,7 +4285,7 @@
       <c r="G119" s="39"/>
       <c r="H119" s="40"/>
     </row>
-    <row r="120" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A120" s="36">
         <v>118</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="G120" s="39"/>
       <c r="H120" s="40"/>
     </row>
-    <row r="121" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A121" s="36">
         <v>119</v>
       </c>
@@ -4331,7 +4331,7 @@
       <c r="G121" s="39"/>
       <c r="H121" s="40"/>
     </row>
-    <row r="122" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A122" s="36">
         <v>120</v>
       </c>
@@ -4361,10 +4361,18 @@
       <c r="B123" s="23">
         <v>4</v>
       </c>
-      <c r="E123" s="18"/>
-      <c r="F123" s="18" t="str">
+      <c r="C123" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D123" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E123" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F123" s="18">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -8515,20 +8523,20 @@
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="18" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="14.453125" style="5"/>
+    <col min="9" max="16384" width="14.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
@@ -8540,7 +8548,7 @@
       <c r="G1" s="50"/>
       <c r="H1" s="50"/>
     </row>
-    <row r="2" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -8566,7 +8574,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>'Bug Metrics'!$A3</f>
         <v>1</v>
@@ -8596,7 +8604,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f>'Bug Metrics'!$A4</f>
         <v>2</v>
@@ -8626,7 +8634,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <f>'Bug Metrics'!$A5</f>
         <v>3</v>
@@ -8656,7 +8664,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <f>'Bug Metrics'!$A6</f>
         <v>4</v>
@@ -8684,7 +8692,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f>'Bug Metrics'!$A7</f>
         <v>5</v>
@@ -8714,7 +8722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f>'Bug Metrics'!$A8</f>
         <v>6</v>
@@ -8744,7 +8752,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f>'Bug Metrics'!$A9</f>
         <v>7</v>
@@ -8774,7 +8782,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f>'Bug Metrics'!$A10</f>
         <v>8</v>
@@ -8804,7 +8812,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <f>'Bug Metrics'!$A11</f>
         <v>9</v>
@@ -8834,7 +8842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <f>'Bug Metrics'!$A12</f>
         <v>10</v>
@@ -8864,7 +8872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <f>'Bug Metrics'!$A13</f>
         <v>11</v>
@@ -8894,7 +8902,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <f>'Bug Metrics'!$A14</f>
         <v>12</v>
@@ -8924,7 +8932,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <f>'Bug Metrics'!$A15</f>
         <v>13</v>
@@ -8954,7 +8962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <f>'Bug Metrics'!$A16</f>
         <v>14</v>
@@ -8984,7 +8992,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <f>'Bug Metrics'!$A17</f>
         <v>15</v>
@@ -9014,7 +9022,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <f>'Bug Metrics'!$A18</f>
         <v>16</v>
@@ -9044,7 +9052,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f>'Bug Metrics'!$A19</f>
         <v>17</v>
@@ -9074,7 +9082,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <f>'Bug Metrics'!$A20</f>
         <v>18</v>
@@ -9104,7 +9112,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <f>'Bug Metrics'!$A21</f>
         <v>19</v>
@@ -9134,7 +9142,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <f>'Bug Metrics'!$A22</f>
         <v>20</v>
@@ -9164,7 +9172,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <f>'Bug Metrics'!$A23</f>
         <v>21</v>
@@ -9194,7 +9202,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <f>'Bug Metrics'!$A24</f>
         <v>22</v>
@@ -9224,7 +9232,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <f>'Bug Metrics'!$A25</f>
         <v>23</v>
@@ -9254,7 +9262,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <f>'Bug Metrics'!$A26</f>
         <v>24</v>
@@ -9284,7 +9292,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <f>'Bug Metrics'!$A27</f>
         <v>25</v>
@@ -9314,7 +9322,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <f>'Bug Metrics'!$A28</f>
         <v>26</v>
@@ -9344,7 +9352,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <f>'Bug Metrics'!$A29</f>
         <v>27</v>
@@ -9374,7 +9382,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <f>'Bug Metrics'!$A30</f>
         <v>28</v>
@@ -9404,7 +9412,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <f>'Bug Metrics'!$A31</f>
         <v>29</v>
@@ -9434,7 +9442,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <f>'Bug Metrics'!$A32</f>
         <v>30</v>
@@ -9464,7 +9472,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <f>'Bug Metrics'!$A33</f>
         <v>31</v>
@@ -9494,7 +9502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <f>'Bug Metrics'!$A34</f>
         <v>32</v>
@@ -9524,7 +9532,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <f>'Bug Metrics'!$A35</f>
         <v>33</v>
@@ -9554,7 +9562,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <f>'Bug Metrics'!$A36</f>
         <v>34</v>
@@ -9584,7 +9592,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="9">
         <f>'Bug Metrics'!$A37</f>
         <v>35</v>
@@ -9614,7 +9622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <f>'Bug Metrics'!$A38</f>
         <v>36</v>
@@ -9644,7 +9652,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <f>'Bug Metrics'!$A39</f>
         <v>37</v>
@@ -9674,7 +9682,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <f>'Bug Metrics'!$A40</f>
         <v>38</v>
@@ -9704,7 +9712,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="9">
         <f>'Bug Metrics'!$B42</f>
@@ -9731,7 +9739,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="9">
         <f>'Bug Metrics'!$B43</f>
@@ -9758,7 +9766,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="9">
         <f>'Bug Metrics'!$B44</f>
@@ -9785,7 +9793,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="9">
         <f>'Bug Metrics'!$B45</f>
@@ -9812,7 +9820,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="9">
         <f>'Bug Metrics'!$B46</f>
@@ -9839,7 +9847,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="9">
         <f>'Bug Metrics'!$B47</f>
@@ -9866,7 +9874,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="9">
         <f>'Bug Metrics'!$B48</f>
@@ -9893,7 +9901,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="9">
         <f>'Bug Metrics'!$B49</f>
@@ -9920,7 +9928,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="9">
         <f>'Bug Metrics'!$B50</f>
@@ -9947,7 +9955,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
       <c r="B50" s="9">
         <f>'Bug Metrics'!$B51</f>
@@ -9974,7 +9982,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="9">
         <f>'Bug Metrics'!$B52</f>
@@ -10001,7 +10009,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="9">
         <f>'Bug Metrics'!$B53</f>
@@ -10028,7 +10036,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="9">
         <v>3</v>
@@ -10054,7 +10062,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="9">
         <f>'Bug Metrics'!$B55</f>
@@ -10077,7 +10085,7 @@
       <c r="G54" s="14"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
       <c r="B55" s="9">
         <f>'Bug Metrics'!$B56</f>
@@ -10100,7 +10108,7 @@
       <c r="G55" s="14"/>
       <c r="H55" s="16"/>
     </row>
-    <row r="56" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="9">
         <f>'Bug Metrics'!$B57</f>
@@ -10123,7 +10131,7 @@
       <c r="G56" s="14"/>
       <c r="H56" s="16"/>
     </row>
-    <row r="57" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
       <c r="B57" s="9">
         <f>'Bug Metrics'!$B58</f>
@@ -10146,7 +10154,7 @@
       <c r="G57" s="14"/>
       <c r="H57" s="16"/>
     </row>
-    <row r="58" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
       <c r="B58" s="9">
         <f>'Bug Metrics'!$B59</f>
@@ -10169,7 +10177,7 @@
       <c r="G58" s="14"/>
       <c r="H58" s="16"/>
     </row>
-    <row r="59" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="9">
         <f>'Bug Metrics'!$B60</f>
@@ -10192,7 +10200,7 @@
       <c r="G59" s="14"/>
       <c r="H59" s="16"/>
     </row>
-    <row r="60" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="9">
         <f>'Bug Metrics'!$B61</f>
@@ -10215,7 +10223,7 @@
       <c r="G60" s="14"/>
       <c r="H60" s="16"/>
     </row>
-    <row r="61" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="9">
         <f>'Bug Metrics'!$B62</f>
@@ -10238,7 +10246,7 @@
       <c r="G61" s="14"/>
       <c r="H61" s="16"/>
     </row>
-    <row r="62" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="9">
         <f>'Bug Metrics'!$B63</f>
@@ -10261,7 +10269,7 @@
       <c r="G62" s="14"/>
       <c r="H62" s="16"/>
     </row>
-    <row r="63" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
       <c r="B63" s="9">
         <f>'Bug Metrics'!$B64</f>
@@ -10284,7 +10292,7 @@
       <c r="G63" s="14"/>
       <c r="H63" s="16"/>
     </row>
-    <row r="64" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
       <c r="B64" s="9">
         <f>'Bug Metrics'!$B65</f>
@@ -10307,7 +10315,7 @@
       <c r="G64" s="14"/>
       <c r="H64" s="16"/>
     </row>
-    <row r="65" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="9"/>
       <c r="B65" s="9">
         <f>'Bug Metrics'!$B66</f>
@@ -10330,7 +10338,7 @@
       <c r="G65" s="14"/>
       <c r="H65" s="16"/>
     </row>
-    <row r="66" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="9">
         <f>'Bug Metrics'!$B67</f>
@@ -10353,7 +10361,7 @@
       <c r="G66" s="14"/>
       <c r="H66" s="16"/>
     </row>
-    <row r="67" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
       <c r="B67" s="9">
         <f>'Bug Metrics'!$B68</f>
@@ -10376,7 +10384,7 @@
       <c r="G67" s="14"/>
       <c r="H67" s="16"/>
     </row>
-    <row r="68" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="9"/>
       <c r="B68" s="9">
         <f>'Bug Metrics'!$B69</f>
@@ -10399,7 +10407,7 @@
       <c r="G68" s="14"/>
       <c r="H68" s="16"/>
     </row>
-    <row r="69" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
       <c r="B69" s="9">
         <f>'Bug Metrics'!$B70</f>
@@ -10422,7 +10430,7 @@
       <c r="G69" s="14"/>
       <c r="H69" s="16"/>
     </row>
-    <row r="70" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="9">
         <f>'Bug Metrics'!$B71</f>
@@ -10445,7 +10453,7 @@
       <c r="G70" s="14"/>
       <c r="H70" s="16"/>
     </row>
-    <row r="71" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="9">
         <f>'Bug Metrics'!$B72</f>
@@ -10468,7 +10476,7 @@
       <c r="G71" s="14"/>
       <c r="H71" s="16"/>
     </row>
-    <row r="72" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
       <c r="B72" s="9">
         <f>'Bug Metrics'!$B73</f>
@@ -10491,7 +10499,7 @@
       <c r="G72" s="14"/>
       <c r="H72" s="16"/>
     </row>
-    <row r="73" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="9">
         <f>'Bug Metrics'!$B74</f>
@@ -10514,7 +10522,7 @@
       <c r="G73" s="14"/>
       <c r="H73" s="16"/>
     </row>
-    <row r="74" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
       <c r="B74" s="9">
         <f>'Bug Metrics'!$B75</f>
@@ -10537,7 +10545,7 @@
       <c r="G74" s="14"/>
       <c r="H74" s="16"/>
     </row>
-    <row r="75" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>
       <c r="B75" s="9">
         <f>'Bug Metrics'!$B76</f>
@@ -10560,7 +10568,7 @@
       <c r="G75" s="14"/>
       <c r="H75" s="16"/>
     </row>
-    <row r="76" spans="1:8" ht="43.8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
       <c r="B76" s="9">
         <f>'Bug Metrics'!$B77</f>
@@ -10583,7 +10591,7 @@
       <c r="G76" s="14"/>
       <c r="H76" s="16"/>
     </row>
-    <row r="77" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A77" s="9"/>
       <c r="B77" s="9">
         <f>'Bug Metrics'!$B78</f>
@@ -10606,7 +10614,7 @@
       <c r="G77" s="14"/>
       <c r="H77" s="16"/>
     </row>
-    <row r="78" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A78" s="9"/>
       <c r="B78" s="9">
         <f>'Bug Metrics'!$B79</f>
@@ -10629,7 +10637,7 @@
       <c r="G78" s="14"/>
       <c r="H78" s="16"/>
     </row>
-    <row r="79" spans="1:8" ht="43.8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="9"/>
       <c r="B79" s="9">
         <f>'Bug Metrics'!$B80</f>
@@ -10652,7 +10660,7 @@
       <c r="G79" s="14"/>
       <c r="H79" s="16"/>
     </row>
-    <row r="80" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="9"/>
       <c r="B80" s="9">
         <f>'Bug Metrics'!$B81</f>
@@ -10675,7 +10683,7 @@
       <c r="G80" s="14"/>
       <c r="H80" s="16"/>
     </row>
-    <row r="81" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="9"/>
       <c r="B81" s="9">
         <f>'Bug Metrics'!$B82</f>
@@ -10698,7 +10706,7 @@
       <c r="G81" s="14"/>
       <c r="H81" s="16"/>
     </row>
-    <row r="82" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A82" s="9"/>
       <c r="B82" s="9">
         <f>'Bug Metrics'!$B83</f>
@@ -10721,7 +10729,7 @@
       <c r="G82" s="14"/>
       <c r="H82" s="16"/>
     </row>
-    <row r="83" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="9"/>
       <c r="B83" s="9">
         <f>'Bug Metrics'!$B84</f>
@@ -10744,7 +10752,7 @@
       <c r="G83" s="14"/>
       <c r="H83" s="16"/>
     </row>
-    <row r="84" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84" s="9"/>
       <c r="B84" s="9">
         <f>'Bug Metrics'!$B85</f>
@@ -10767,7 +10775,7 @@
       <c r="G84" s="14"/>
       <c r="H84" s="16"/>
     </row>
-    <row r="85" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="B85" s="9">
         <f>'Bug Metrics'!$B86</f>
@@ -10790,7 +10798,7 @@
       <c r="G85" s="14"/>
       <c r="H85" s="16"/>
     </row>
-    <row r="86" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
       <c r="B86" s="9">
         <f>'Bug Metrics'!$B87</f>
@@ -10813,7 +10821,7 @@
       <c r="G86" s="14"/>
       <c r="H86" s="16"/>
     </row>
-    <row r="87" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="9"/>
       <c r="B87" s="9">
         <f>'Bug Metrics'!$B88</f>
@@ -10836,7 +10844,7 @@
       <c r="G87" s="14"/>
       <c r="H87" s="16"/>
     </row>
-    <row r="88" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="9"/>
       <c r="B88" s="9">
         <f>'Bug Metrics'!$B89</f>
@@ -10859,7 +10867,7 @@
       <c r="G88" s="14"/>
       <c r="H88" s="16"/>
     </row>
-    <row r="89" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89" s="9"/>
       <c r="B89" s="9">
         <f>'Bug Metrics'!$B90</f>
@@ -10882,7 +10890,7 @@
       <c r="G89" s="14"/>
       <c r="H89" s="16"/>
     </row>
-    <row r="90" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A90" s="9"/>
       <c r="B90" s="9">
         <f>'Bug Metrics'!$B91</f>
@@ -10905,7 +10913,7 @@
       <c r="G90" s="14"/>
       <c r="H90" s="16"/>
     </row>
-    <row r="91" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A91" s="9"/>
       <c r="B91" s="9">
         <f>'Bug Metrics'!$B92</f>
@@ -10928,7 +10936,7 @@
       <c r="G91" s="14"/>
       <c r="H91" s="16"/>
     </row>
-    <row r="92" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A92" s="9"/>
       <c r="B92" s="9">
         <f>'Bug Metrics'!$B93</f>
@@ -10951,7 +10959,7 @@
       <c r="G92" s="14"/>
       <c r="H92" s="16"/>
     </row>
-    <row r="93" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
       <c r="B93" s="9">
         <f>'Bug Metrics'!$B94</f>
@@ -10974,7 +10982,7 @@
       <c r="G93" s="14"/>
       <c r="H93" s="16"/>
     </row>
-    <row r="94" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="9">
         <f>'Bug Metrics'!$B95</f>
@@ -10997,7 +11005,7 @@
       <c r="G94" s="14"/>
       <c r="H94" s="16"/>
     </row>
-    <row r="95" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
       <c r="B95" s="9">
         <f>'Bug Metrics'!$B96</f>
@@ -11020,7 +11028,7 @@
       <c r="G95" s="14"/>
       <c r="H95" s="16"/>
     </row>
-    <row r="96" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="9"/>
       <c r="B96" s="9">
         <f>'Bug Metrics'!$B97</f>
@@ -11043,7 +11051,7 @@
       <c r="G96" s="14"/>
       <c r="H96" s="16"/>
     </row>
-    <row r="97" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="9"/>
       <c r="B97" s="9">
         <f>'Bug Metrics'!$B98</f>
@@ -11066,7 +11074,7 @@
       <c r="G97" s="14"/>
       <c r="H97" s="16"/>
     </row>
-    <row r="98" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="9"/>
       <c r="B98" s="9">
         <f>'Bug Metrics'!$B99</f>
@@ -11089,7 +11097,7 @@
       <c r="G98" s="14"/>
       <c r="H98" s="16"/>
     </row>
-    <row r="99" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="9"/>
       <c r="B99" s="9">
         <f>'Bug Metrics'!$B100</f>
@@ -11112,7 +11120,7 @@
       <c r="G99" s="14"/>
       <c r="H99" s="16"/>
     </row>
-    <row r="100" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="9"/>
       <c r="B100" s="9">
         <f>'Bug Metrics'!$B101</f>
@@ -11135,7 +11143,7 @@
       <c r="G100" s="14"/>
       <c r="H100" s="16"/>
     </row>
-    <row r="101" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101" s="9"/>
       <c r="B101" s="9">
         <f>'Bug Metrics'!$B102</f>
@@ -11158,7 +11166,7 @@
       <c r="G101" s="14"/>
       <c r="H101" s="16"/>
     </row>
-    <row r="102" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="9"/>
       <c r="B102" s="9">
         <f>'Bug Metrics'!$B103</f>
@@ -11181,7 +11189,7 @@
       <c r="G102" s="14"/>
       <c r="H102" s="16"/>
     </row>
-    <row r="103" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A103" s="9"/>
       <c r="B103" s="9">
         <f>'Bug Metrics'!$B104</f>
@@ -11204,7 +11212,7 @@
       <c r="G103" s="14"/>
       <c r="H103" s="16"/>
     </row>
-    <row r="104" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A104" s="9"/>
       <c r="B104" s="9">
         <f>'Bug Metrics'!$B105</f>
@@ -11227,7 +11235,7 @@
       <c r="G104" s="14"/>
       <c r="H104" s="16"/>
     </row>
-    <row r="105" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A105" s="9"/>
       <c r="B105" s="9">
         <f>'Bug Metrics'!$B106</f>
@@ -11250,7 +11258,7 @@
       <c r="G105" s="14"/>
       <c r="H105" s="16"/>
     </row>
-    <row r="106" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="9"/>
       <c r="B106" s="9">
         <f>'Bug Metrics'!$B107</f>
@@ -11273,7 +11281,7 @@
       <c r="G106" s="14"/>
       <c r="H106" s="16"/>
     </row>
-    <row r="107" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="9"/>
       <c r="B107" s="9">
         <f>'Bug Metrics'!$B108</f>
@@ -11296,7 +11304,7 @@
       <c r="G107" s="14"/>
       <c r="H107" s="16"/>
     </row>
-    <row r="108" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="9"/>
       <c r="B108" s="9">
         <f>'Bug Metrics'!$B109</f>
@@ -11319,7 +11327,7 @@
       <c r="G108" s="14"/>
       <c r="H108" s="16"/>
     </row>
-    <row r="109" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="9"/>
       <c r="B109" s="9">
         <f>'Bug Metrics'!$B110</f>
@@ -11342,7 +11350,7 @@
       <c r="G109" s="14"/>
       <c r="H109" s="16"/>
     </row>
-    <row r="110" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="9"/>
       <c r="B110" s="9">
         <f>'Bug Metrics'!$B111</f>
@@ -11365,7 +11373,7 @@
       <c r="G110" s="14"/>
       <c r="H110" s="16"/>
     </row>
-    <row r="111" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A111" s="9"/>
       <c r="B111" s="9">
         <f>'Bug Metrics'!$B112</f>
@@ -11388,7 +11396,7 @@
       <c r="G111" s="14"/>
       <c r="H111" s="16"/>
     </row>
-    <row r="112" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112" s="9"/>
       <c r="B112" s="9">
         <f>'Bug Metrics'!$B113</f>
@@ -11411,7 +11419,7 @@
       <c r="G112" s="14"/>
       <c r="H112" s="16"/>
     </row>
-    <row r="113" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="9"/>
       <c r="B113" s="9">
         <f>'Bug Metrics'!$B114</f>
@@ -11434,7 +11442,7 @@
       <c r="G113" s="14"/>
       <c r="H113" s="16"/>
     </row>
-    <row r="114" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="9"/>
       <c r="B114" s="9">
         <f>'Bug Metrics'!$B115</f>
@@ -11457,7 +11465,7 @@
       <c r="G114" s="14"/>
       <c r="H114" s="16"/>
     </row>
-    <row r="115" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A115" s="9"/>
       <c r="B115" s="9">
         <f>'Bug Metrics'!$B116</f>
@@ -11480,7 +11488,7 @@
       <c r="G115" s="14"/>
       <c r="H115" s="16"/>
     </row>
-    <row r="116" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116" s="9"/>
       <c r="B116" s="9">
         <f>'Bug Metrics'!$B117</f>
@@ -11503,7 +11511,7 @@
       <c r="G116" s="14"/>
       <c r="H116" s="16"/>
     </row>
-    <row r="117" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A117" s="9"/>
       <c r="B117" s="9">
         <f>'Bug Metrics'!$B118</f>
@@ -11526,7 +11534,7 @@
       <c r="G117" s="14"/>
       <c r="H117" s="16"/>
     </row>
-    <row r="118" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118" s="9"/>
       <c r="B118" s="9">
         <f>'Bug Metrics'!$B119</f>
@@ -11549,7 +11557,7 @@
       <c r="G118" s="14"/>
       <c r="H118" s="16"/>
     </row>
-    <row r="119" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A119" s="9"/>
       <c r="B119" s="9">
         <f>'Bug Metrics'!$B120</f>
@@ -11572,7 +11580,7 @@
       <c r="G119" s="14"/>
       <c r="H119" s="16"/>
     </row>
-    <row r="120" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A120" s="9"/>
       <c r="B120" s="9">
         <f>'Bug Metrics'!$B121</f>
@@ -11595,7 +11603,7 @@
       <c r="G120" s="14"/>
       <c r="H120" s="16"/>
     </row>
-    <row r="121" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A121" s="9"/>
       <c r="B121" s="9">
         <f>'Bug Metrics'!$B122</f>
@@ -11618,7 +11626,7 @@
       <c r="G121" s="14"/>
       <c r="H121" s="16"/>
     </row>
-    <row r="122" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="9"/>
       <c r="B122" s="9">
         <f>'Bug Metrics'!$B123</f>
@@ -11641,7 +11649,7 @@
       <c r="G122" s="14"/>
       <c r="H122" s="16"/>
     </row>
-    <row r="123" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A123" s="9"/>
       <c r="B123" s="9">
         <f>'Bug Metrics'!$B124</f>
@@ -11654,7 +11662,7 @@
       <c r="G123" s="14"/>
       <c r="H123" s="16"/>
     </row>
-    <row r="124" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A124" s="9"/>
       <c r="B124" s="9">
         <f>'Bug Metrics'!$B125</f>
@@ -11667,7 +11675,7 @@
       <c r="G124" s="14"/>
       <c r="H124" s="16"/>
     </row>
-    <row r="125" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A125" s="9"/>
       <c r="B125" s="9">
         <f>'Bug Metrics'!$B126</f>
@@ -11680,7 +11688,7 @@
       <c r="G125" s="14"/>
       <c r="H125" s="16"/>
     </row>
-    <row r="126" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A126" s="9"/>
       <c r="B126" s="9">
         <f>'Bug Metrics'!$B127</f>
@@ -11693,7 +11701,7 @@
       <c r="G126" s="14"/>
       <c r="H126" s="16"/>
     </row>
-    <row r="127" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A127" s="9"/>
       <c r="B127" s="9">
         <f>'Bug Metrics'!$B128</f>
@@ -11706,7 +11714,7 @@
       <c r="G127" s="14"/>
       <c r="H127" s="16"/>
     </row>
-    <row r="128" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A128" s="9"/>
       <c r="B128" s="9">
         <f>'Bug Metrics'!$B129</f>
@@ -11719,7 +11727,7 @@
       <c r="G128" s="14"/>
       <c r="H128" s="16"/>
     </row>
-    <row r="129" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A129" s="9"/>
       <c r="B129" s="9">
         <f>'Bug Metrics'!$B130</f>
@@ -11732,7 +11740,7 @@
       <c r="G129" s="14"/>
       <c r="H129" s="16"/>
     </row>
-    <row r="130" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A130" s="9"/>
       <c r="B130" s="9">
         <f>'Bug Metrics'!$B131</f>
@@ -11745,7 +11753,7 @@
       <c r="G130" s="14"/>
       <c r="H130" s="16"/>
     </row>
-    <row r="131" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A131" s="9"/>
       <c r="B131" s="9">
         <f>'Bug Metrics'!$B132</f>
@@ -11758,7 +11766,7 @@
       <c r="G131" s="14"/>
       <c r="H131" s="16"/>
     </row>
-    <row r="132" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A132" s="9"/>
       <c r="B132" s="9">
         <f>'Bug Metrics'!$B133</f>
@@ -11771,7 +11779,7 @@
       <c r="G132" s="14"/>
       <c r="H132" s="16"/>
     </row>
-    <row r="133" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A133" s="9"/>
       <c r="B133" s="9">
         <f>'Bug Metrics'!$B134</f>
@@ -11784,7 +11792,7 @@
       <c r="G133" s="14"/>
       <c r="H133" s="16"/>
     </row>
-    <row r="134" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A134" s="9"/>
       <c r="B134" s="9">
         <f>'Bug Metrics'!$B135</f>
@@ -11797,7 +11805,7 @@
       <c r="G134" s="14"/>
       <c r="H134" s="16"/>
     </row>
-    <row r="135" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A135" s="9"/>
       <c r="B135" s="9">
         <f>'Bug Metrics'!$B136</f>
@@ -11810,7 +11818,7 @@
       <c r="G135" s="14"/>
       <c r="H135" s="16"/>
     </row>
-    <row r="136" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A136" s="9"/>
       <c r="B136" s="9">
         <f>'Bug Metrics'!$B137</f>
@@ -11823,7 +11831,7 @@
       <c r="G136" s="14"/>
       <c r="H136" s="16"/>
     </row>
-    <row r="137" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A137" s="9"/>
       <c r="B137" s="9">
         <f>'Bug Metrics'!$B138</f>
@@ -11836,7 +11844,7 @@
       <c r="G137" s="14"/>
       <c r="H137" s="16"/>
     </row>
-    <row r="138" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A138" s="9"/>
       <c r="B138" s="9">
         <f>'Bug Metrics'!$B139</f>
@@ -11849,7 +11857,7 @@
       <c r="G138" s="14"/>
       <c r="H138" s="16"/>
     </row>
-    <row r="139" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A139" s="9"/>
       <c r="B139" s="9">
         <f>'Bug Metrics'!$B140</f>
@@ -11862,7 +11870,7 @@
       <c r="G139" s="14"/>
       <c r="H139" s="16"/>
     </row>
-    <row r="140" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A140" s="9"/>
       <c r="B140" s="9">
         <f>'Bug Metrics'!$B141</f>
@@ -11875,7 +11883,7 @@
       <c r="G140" s="14"/>
       <c r="H140" s="16"/>
     </row>
-    <row r="141" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A141" s="9"/>
       <c r="B141" s="9">
         <f>'Bug Metrics'!$B142</f>
@@ -11888,7 +11896,7 @@
       <c r="G141" s="14"/>
       <c r="H141" s="16"/>
     </row>
-    <row r="142" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A142" s="9"/>
       <c r="B142" s="9">
         <f>'Bug Metrics'!$B143</f>
@@ -11901,7 +11909,7 @@
       <c r="G142" s="14"/>
       <c r="H142" s="16"/>
     </row>
-    <row r="143" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A143" s="9"/>
       <c r="B143" s="9">
         <f>'Bug Metrics'!$B144</f>
@@ -11914,7 +11922,7 @@
       <c r="G143" s="14"/>
       <c r="H143" s="16"/>
     </row>
-    <row r="144" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A144" s="9"/>
       <c r="B144" s="9">
         <f>'Bug Metrics'!$B145</f>
@@ -11927,7 +11935,7 @@
       <c r="G144" s="14"/>
       <c r="H144" s="16"/>
     </row>
-    <row r="145" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A145" s="9"/>
       <c r="B145" s="9">
         <f>'Bug Metrics'!$B146</f>
@@ -11940,7 +11948,7 @@
       <c r="G145" s="14"/>
       <c r="H145" s="16"/>
     </row>
-    <row r="146" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A146" s="9"/>
       <c r="B146" s="9">
         <f>'Bug Metrics'!$B147</f>
@@ -11953,7 +11961,7 @@
       <c r="G146" s="14"/>
       <c r="H146" s="16"/>
     </row>
-    <row r="147" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A147" s="9"/>
       <c r="B147" s="9">
         <f>'Bug Metrics'!$B148</f>
@@ -11966,7 +11974,7 @@
       <c r="G147" s="14"/>
       <c r="H147" s="16"/>
     </row>
-    <row r="148" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A148" s="9"/>
       <c r="B148" s="9">
         <f>'Bug Metrics'!$B149</f>
@@ -11979,7 +11987,7 @@
       <c r="G148" s="14"/>
       <c r="H148" s="16"/>
     </row>
-    <row r="149" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A149" s="9"/>
       <c r="B149" s="9">
         <f>'Bug Metrics'!$B150</f>
@@ -11992,7 +12000,7 @@
       <c r="G149" s="14"/>
       <c r="H149" s="16"/>
     </row>
-    <row r="150" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A150" s="9"/>
       <c r="B150" s="9">
         <f>'Bug Metrics'!$B151</f>
@@ -12005,7 +12013,7 @@
       <c r="G150" s="14"/>
       <c r="H150" s="16"/>
     </row>
-    <row r="151" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A151" s="9"/>
       <c r="B151" s="9">
         <f>'Bug Metrics'!$B152</f>
@@ -12018,7 +12026,7 @@
       <c r="G151" s="14"/>
       <c r="H151" s="16"/>
     </row>
-    <row r="152" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A152" s="9"/>
       <c r="B152" s="9">
         <f>'Bug Metrics'!$B153</f>
@@ -12031,7 +12039,7 @@
       <c r="G152" s="14"/>
       <c r="H152" s="16"/>
     </row>
-    <row r="153" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A153" s="9"/>
       <c r="B153" s="9">
         <f>'Bug Metrics'!$B154</f>
@@ -12044,7 +12052,7 @@
       <c r="G153" s="14"/>
       <c r="H153" s="16"/>
     </row>
-    <row r="154" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A154" s="9"/>
       <c r="B154" s="9">
         <f>'Bug Metrics'!$B155</f>
@@ -12057,7 +12065,7 @@
       <c r="G154" s="14"/>
       <c r="H154" s="16"/>
     </row>
-    <row r="155" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A155" s="9"/>
       <c r="B155" s="9">
         <f>'Bug Metrics'!$B156</f>
@@ -12070,7 +12078,7 @@
       <c r="G155" s="14"/>
       <c r="H155" s="16"/>
     </row>
-    <row r="156" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A156" s="9"/>
       <c r="B156" s="9">
         <f>'Bug Metrics'!$B157</f>
@@ -12083,7 +12091,7 @@
       <c r="G156" s="14"/>
       <c r="H156" s="16"/>
     </row>
-    <row r="157" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A157" s="9"/>
       <c r="B157" s="9">
         <f>'Bug Metrics'!$B158</f>
@@ -12096,7 +12104,7 @@
       <c r="G157" s="14"/>
       <c r="H157" s="16"/>
     </row>
-    <row r="158" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A158" s="9"/>
       <c r="B158" s="9">
         <f>'Bug Metrics'!$B159</f>
@@ -12109,7 +12117,7 @@
       <c r="G158" s="14"/>
       <c r="H158" s="16"/>
     </row>
-    <row r="159" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A159" s="9"/>
       <c r="B159" s="9">
         <f>'Bug Metrics'!$B160</f>
@@ -12122,7 +12130,7 @@
       <c r="G159" s="14"/>
       <c r="H159" s="16"/>
     </row>
-    <row r="160" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A160" s="9"/>
       <c r="B160" s="9">
         <f>'Bug Metrics'!$B161</f>
@@ -12135,7 +12143,7 @@
       <c r="G160" s="14"/>
       <c r="H160" s="16"/>
     </row>
-    <row r="161" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A161" s="9"/>
       <c r="B161" s="9">
         <f>'Bug Metrics'!$B162</f>
@@ -12148,7 +12156,7 @@
       <c r="G161" s="14"/>
       <c r="H161" s="16"/>
     </row>
-    <row r="162" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A162" s="9"/>
       <c r="B162" s="9">
         <f>'Bug Metrics'!$B163</f>
@@ -12161,7 +12169,7 @@
       <c r="G162" s="14"/>
       <c r="H162" s="16"/>
     </row>
-    <row r="163" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A163" s="9"/>
       <c r="B163" s="9">
         <f>'Bug Metrics'!$B164</f>
@@ -12174,7 +12182,7 @@
       <c r="G163" s="14"/>
       <c r="H163" s="16"/>
     </row>
-    <row r="164" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A164" s="9"/>
       <c r="B164" s="9">
         <f>'Bug Metrics'!$B165</f>
@@ -12187,7 +12195,7 @@
       <c r="G164" s="14"/>
       <c r="H164" s="16"/>
     </row>
-    <row r="165" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A165" s="9"/>
       <c r="B165" s="9">
         <f>'Bug Metrics'!$B166</f>
@@ -12200,7 +12208,7 @@
       <c r="G165" s="14"/>
       <c r="H165" s="16"/>
     </row>
-    <row r="166" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A166" s="9"/>
       <c r="B166" s="9">
         <f>'Bug Metrics'!$B167</f>
@@ -12213,7 +12221,7 @@
       <c r="G166" s="14"/>
       <c r="H166" s="16"/>
     </row>
-    <row r="167" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A167" s="9"/>
       <c r="B167" s="9">
         <f>'Bug Metrics'!$B168</f>
@@ -12226,7 +12234,7 @@
       <c r="G167" s="14"/>
       <c r="H167" s="16"/>
     </row>
-    <row r="168" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A168" s="9"/>
       <c r="B168" s="9">
         <f>'Bug Metrics'!$B169</f>
@@ -12239,7 +12247,7 @@
       <c r="G168" s="14"/>
       <c r="H168" s="16"/>
     </row>
-    <row r="169" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A169" s="9"/>
       <c r="B169" s="9">
         <f>'Bug Metrics'!$B170</f>
@@ -12252,7 +12260,7 @@
       <c r="G169" s="14"/>
       <c r="H169" s="16"/>
     </row>
-    <row r="170" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A170" s="9"/>
       <c r="B170" s="9">
         <f>'Bug Metrics'!$B171</f>
@@ -12265,7 +12273,7 @@
       <c r="G170" s="14"/>
       <c r="H170" s="16"/>
     </row>
-    <row r="171" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A171" s="9"/>
       <c r="B171" s="9">
         <f>'Bug Metrics'!$B172</f>
@@ -12278,7 +12286,7 @@
       <c r="G171" s="14"/>
       <c r="H171" s="16"/>
     </row>
-    <row r="172" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A172" s="9"/>
       <c r="B172" s="9">
         <f>'Bug Metrics'!$B173</f>
@@ -12291,7 +12299,7 @@
       <c r="G172" s="14"/>
       <c r="H172" s="16"/>
     </row>
-    <row r="173" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A173" s="9"/>
       <c r="B173" s="9">
         <f>'Bug Metrics'!$B174</f>
@@ -12304,7 +12312,7 @@
       <c r="G173" s="14"/>
       <c r="H173" s="16"/>
     </row>
-    <row r="174" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A174" s="9"/>
       <c r="B174" s="9">
         <f>'Bug Metrics'!$B175</f>
@@ -12317,7 +12325,7 @@
       <c r="G174" s="14"/>
       <c r="H174" s="16"/>
     </row>
-    <row r="175" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A175" s="9"/>
       <c r="B175" s="9">
         <f>'Bug Metrics'!$B176</f>
@@ -12330,7 +12338,7 @@
       <c r="G175" s="14"/>
       <c r="H175" s="16"/>
     </row>
-    <row r="176" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A176" s="9"/>
       <c r="B176" s="9">
         <f>'Bug Metrics'!$B177</f>
@@ -12343,7 +12351,7 @@
       <c r="G176" s="14"/>
       <c r="H176" s="16"/>
     </row>
-    <row r="177" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A177" s="9"/>
       <c r="B177" s="9">
         <f>'Bug Metrics'!$B178</f>
@@ -12356,7 +12364,7 @@
       <c r="G177" s="14"/>
       <c r="H177" s="16"/>
     </row>
-    <row r="178" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A178" s="9"/>
       <c r="B178" s="9">
         <f>'Bug Metrics'!$B179</f>
@@ -12369,7 +12377,7 @@
       <c r="G178" s="14"/>
       <c r="H178" s="16"/>
     </row>
-    <row r="179" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A179" s="9"/>
       <c r="B179" s="9">
         <f>'Bug Metrics'!$B180</f>
@@ -12382,7 +12390,7 @@
       <c r="G179" s="14"/>
       <c r="H179" s="16"/>
     </row>
-    <row r="180" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A180" s="9"/>
       <c r="B180" s="9">
         <f>'Bug Metrics'!$B181</f>
@@ -12395,7 +12403,7 @@
       <c r="G180" s="14"/>
       <c r="H180" s="16"/>
     </row>
-    <row r="181" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A181" s="9"/>
       <c r="B181" s="9">
         <f>'Bug Metrics'!$B182</f>
@@ -12408,7 +12416,7 @@
       <c r="G181" s="14"/>
       <c r="H181" s="16"/>
     </row>
-    <row r="182" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A182" s="9"/>
       <c r="B182" s="9">
         <f>'Bug Metrics'!$B183</f>
@@ -12421,7 +12429,7 @@
       <c r="G182" s="14"/>
       <c r="H182" s="16"/>
     </row>
-    <row r="183" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A183" s="9"/>
       <c r="B183" s="9">
         <f>'Bug Metrics'!$B184</f>
@@ -12434,7 +12442,7 @@
       <c r="G183" s="14"/>
       <c r="H183" s="16"/>
     </row>
-    <row r="184" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A184" s="9"/>
       <c r="B184" s="9">
         <f>'Bug Metrics'!$B185</f>
@@ -12447,7 +12455,7 @@
       <c r="G184" s="14"/>
       <c r="H184" s="16"/>
     </row>
-    <row r="185" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A185" s="9"/>
       <c r="B185" s="9">
         <f>'Bug Metrics'!$B186</f>
@@ -12460,7 +12468,7 @@
       <c r="G185" s="14"/>
       <c r="H185" s="16"/>
     </row>
-    <row r="186" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A186" s="9"/>
       <c r="B186" s="9">
         <f>'Bug Metrics'!$B187</f>
@@ -12473,7 +12481,7 @@
       <c r="G186" s="14"/>
       <c r="H186" s="16"/>
     </row>
-    <row r="187" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A187" s="9"/>
       <c r="B187" s="9">
         <f>'Bug Metrics'!$B188</f>
@@ -12486,7 +12494,7 @@
       <c r="G187" s="14"/>
       <c r="H187" s="16"/>
     </row>
-    <row r="188" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A188" s="9"/>
       <c r="B188" s="9">
         <f>'Bug Metrics'!$B189</f>
@@ -12499,7 +12507,7 @@
       <c r="G188" s="14"/>
       <c r="H188" s="16"/>
     </row>
-    <row r="189" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A189" s="9"/>
       <c r="B189" s="9">
         <f>'Bug Metrics'!$B190</f>
@@ -12512,7 +12520,7 @@
       <c r="G189" s="14"/>
       <c r="H189" s="16"/>
     </row>
-    <row r="190" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A190" s="9"/>
       <c r="B190" s="9">
         <f>'Bug Metrics'!$B191</f>
@@ -12525,7 +12533,7 @@
       <c r="G190" s="14"/>
       <c r="H190" s="16"/>
     </row>
-    <row r="191" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A191" s="9"/>
       <c r="B191" s="9">
         <f>'Bug Metrics'!$B192</f>
@@ -12538,7 +12546,7 @@
       <c r="G191" s="14"/>
       <c r="H191" s="16"/>
     </row>
-    <row r="192" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A192" s="9"/>
       <c r="B192" s="9">
         <f>'Bug Metrics'!$B193</f>
@@ -12551,7 +12559,7 @@
       <c r="G192" s="14"/>
       <c r="H192" s="16"/>
     </row>
-    <row r="193" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A193" s="9"/>
       <c r="B193" s="9">
         <f>'Bug Metrics'!$B194</f>
@@ -12564,7 +12572,7 @@
       <c r="G193" s="14"/>
       <c r="H193" s="16"/>
     </row>
-    <row r="194" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A194" s="9"/>
       <c r="B194" s="9">
         <f>'Bug Metrics'!$B195</f>
@@ -12577,7 +12585,7 @@
       <c r="G194" s="14"/>
       <c r="H194" s="16"/>
     </row>
-    <row r="195" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A195" s="9"/>
       <c r="B195" s="9">
         <f>'Bug Metrics'!$B196</f>
@@ -12590,7 +12598,7 @@
       <c r="G195" s="14"/>
       <c r="H195" s="16"/>
     </row>
-    <row r="196" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A196" s="9"/>
       <c r="B196" s="9">
         <f>'Bug Metrics'!$B197</f>
@@ -12603,7 +12611,7 @@
       <c r="G196" s="14"/>
       <c r="H196" s="16"/>
     </row>
-    <row r="197" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A197" s="9"/>
       <c r="B197" s="9">
         <f>'Bug Metrics'!$B198</f>
@@ -12616,7 +12624,7 @@
       <c r="G197" s="14"/>
       <c r="H197" s="16"/>
     </row>
-    <row r="198" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A198" s="9"/>
       <c r="B198" s="9">
         <f>'Bug Metrics'!$B199</f>
@@ -12629,7 +12637,7 @@
       <c r="G198" s="14"/>
       <c r="H198" s="16"/>
     </row>
-    <row r="199" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A199" s="9"/>
       <c r="B199" s="9">
         <f>'Bug Metrics'!$B200</f>
@@ -12642,7 +12650,7 @@
       <c r="G199" s="14"/>
       <c r="H199" s="16"/>
     </row>
-    <row r="200" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A200" s="9"/>
       <c r="B200" s="9">
         <f>'Bug Metrics'!$B201</f>
@@ -12655,7 +12663,7 @@
       <c r="G200" s="14"/>
       <c r="H200" s="16"/>
     </row>
-    <row r="201" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
       <c r="B201" s="9"/>
       <c r="C201" s="13"/>
@@ -12665,7 +12673,7 @@
       <c r="G201" s="14"/>
       <c r="H201" s="13"/>
     </row>
-    <row r="202" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A202" s="13"/>
       <c r="B202" s="9"/>
       <c r="C202" s="13"/>
@@ -12675,7 +12683,7 @@
       <c r="G202" s="14"/>
       <c r="H202" s="13"/>
     </row>
-    <row r="203" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A203" s="13"/>
       <c r="B203" s="9"/>
       <c r="C203" s="13"/>
@@ -20720,32 +20728,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E32 E34:E200">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E32 E34:E200">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E32 E34:E200">
-    <cfRule type="containsBlanks" dxfId="0" priority="6">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(E33))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
debugged errors caused by repository merging
Co-Authored-By: j1em1n <j1em1n@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\GitHub\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22160B8D-F0A9-4601-9311-080B3BC0F26B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2167CA-DDB2-443C-8D91-1713EE09CD3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="236">
   <si>
     <t>Bug Log</t>
   </si>
@@ -735,6 +735,12 @@
   </si>
   <si>
     <t>ST &amp; JM</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Information about round number, status and student edollar balance is repeated on home page</t>
   </si>
 </sst>
 </file>
@@ -991,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1103,14 +1109,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1124,22 +1142,13 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1763,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1005"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" zoomScale="72" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123:H176"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="72" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123:G178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.6" x14ac:dyDescent="0.25"/>
@@ -1782,16 +1791,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -1838,11 +1847,11 @@
       <c r="F3" s="25">
         <v>5</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="44">
         <f>SUM(F3:F7)</f>
         <v>26</v>
       </c>
-      <c r="H3" s="47" t="str">
+      <c r="H3" s="40" t="str">
         <f xml:space="preserve"> IF(G3&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1866,8 +1875,8 @@
       <c r="F4" s="25">
         <v>1</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="48"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
@@ -1888,8 +1897,8 @@
       <c r="F5" s="25">
         <v>5</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="48"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
@@ -1910,8 +1919,8 @@
       <c r="F6" s="25">
         <v>5</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="48"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
@@ -1932,8 +1941,8 @@
       <c r="F7" s="25">
         <v>10</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="49"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="25">
@@ -1954,11 +1963,11 @@
       <c r="F8" s="25">
         <v>5</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="47">
         <f>SUM(F8:F32)</f>
         <v>156</v>
       </c>
-      <c r="H8" s="44" t="str">
+      <c r="H8" s="48" t="str">
         <f xml:space="preserve"> IF(G8&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1982,8 +1991,8 @@
       <c r="F9" s="25">
         <v>5</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="45"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="25">
@@ -2004,8 +2013,8 @@
       <c r="F10" s="25">
         <v>5</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="45"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="25">
@@ -2026,8 +2035,8 @@
       <c r="F11" s="25">
         <v>10</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="45"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="49"/>
     </row>
     <row r="12" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25">
@@ -2048,8 +2057,8 @@
       <c r="F12" s="25">
         <v>10</v>
       </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="45"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="49"/>
     </row>
     <row r="13" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="25">
@@ -2070,8 +2079,8 @@
       <c r="F13" s="25">
         <v>10</v>
       </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="45"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25">
@@ -2092,8 +2101,8 @@
       <c r="F14" s="25">
         <v>10</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="45"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="49"/>
     </row>
     <row r="15" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="25">
@@ -2114,8 +2123,8 @@
       <c r="F15" s="25">
         <v>10</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="45"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="49"/>
     </row>
     <row r="16" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="29">
@@ -2136,8 +2145,8 @@
       <c r="F16" s="25">
         <v>5</v>
       </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="45"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="49"/>
     </row>
     <row r="17" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="30">
@@ -2158,8 +2167,8 @@
       <c r="F17" s="25">
         <v>1</v>
       </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="45"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="49"/>
     </row>
     <row r="18" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="30">
@@ -2180,8 +2189,8 @@
       <c r="F18" s="25">
         <v>5</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="45"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="31">
@@ -2202,8 +2211,8 @@
       <c r="F19" s="25">
         <v>1</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="45"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="49"/>
     </row>
     <row r="20" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="18">
@@ -2225,8 +2234,8 @@
         <f t="shared" ref="F20:F187" si="0">IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="45"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="18">
@@ -2248,8 +2257,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="45"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18">
@@ -2271,8 +2280,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="45"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="18">
@@ -2294,8 +2303,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="45"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="18">
@@ -2317,8 +2326,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="45"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="18">
@@ -2340,8 +2349,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G25" s="43"/>
-      <c r="H25" s="45"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="18">
@@ -2363,8 +2372,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="45"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="18">
@@ -2386,8 +2395,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G27" s="43"/>
-      <c r="H27" s="45"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="18">
@@ -2409,8 +2418,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G28" s="43"/>
-      <c r="H28" s="45"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18">
@@ -2432,8 +2441,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G29" s="43"/>
-      <c r="H29" s="45"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="18">
@@ -2455,8 +2464,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="45"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="49"/>
     </row>
     <row r="31" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="18">
@@ -2478,8 +2487,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G31" s="43"/>
-      <c r="H31" s="45"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="49"/>
     </row>
     <row r="32" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="18">
@@ -2501,8 +2510,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="45"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="49"/>
     </row>
     <row r="33" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -2524,11 +2533,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G33" s="41">
+      <c r="G33" s="43">
         <f>SUM(F33:F53)</f>
         <v>142</v>
       </c>
-      <c r="H33" s="42" t="str">
+      <c r="H33" s="46" t="str">
         <f xml:space="preserve"> IF(G33&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -2553,8 +2562,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G34" s="41"/>
-      <c r="H34" s="42"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="46"/>
     </row>
     <row r="35" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
@@ -2576,8 +2585,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G35" s="41"/>
-      <c r="H35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="46"/>
     </row>
     <row r="36" spans="1:8" ht="23.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18">
@@ -2599,8 +2608,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G36" s="41"/>
-      <c r="H36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="46"/>
     </row>
     <row r="37" spans="1:8" ht="23.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18">
@@ -2622,8 +2631,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G37" s="41"/>
-      <c r="H37" s="42"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="46"/>
     </row>
     <row r="38" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
@@ -2645,8 +2654,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G38" s="41"/>
-      <c r="H38" s="42"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="46"/>
     </row>
     <row r="39" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18">
@@ -2668,8 +2677,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G39" s="41"/>
-      <c r="H39" s="42"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="46"/>
     </row>
     <row r="40" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
@@ -2691,8 +2700,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G40" s="41"/>
-      <c r="H40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="46"/>
     </row>
     <row r="41" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18">
@@ -2714,8 +2723,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G41" s="41"/>
-      <c r="H41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="46"/>
     </row>
     <row r="42" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -2737,8 +2746,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G42" s="41"/>
-      <c r="H42" s="42"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="46"/>
     </row>
     <row r="43" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -2760,8 +2769,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G43" s="41"/>
-      <c r="H43" s="42"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="46"/>
     </row>
     <row r="44" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18">
@@ -2783,8 +2792,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G44" s="41"/>
-      <c r="H44" s="42"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="46"/>
     </row>
     <row r="45" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18">
@@ -2806,8 +2815,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G45" s="41"/>
-      <c r="H45" s="42"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="46"/>
     </row>
     <row r="46" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18">
@@ -2829,8 +2838,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G46" s="41"/>
-      <c r="H46" s="42"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="46"/>
     </row>
     <row r="47" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -2852,8 +2861,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G47" s="41"/>
-      <c r="H47" s="42"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="46"/>
     </row>
     <row r="48" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -2875,8 +2884,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G48" s="41"/>
-      <c r="H48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="46"/>
     </row>
     <row r="49" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -2898,8 +2907,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G49" s="41"/>
-      <c r="H49" s="42"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="46"/>
     </row>
     <row r="50" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -2921,8 +2930,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G50" s="41"/>
-      <c r="H50" s="42"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="46"/>
     </row>
     <row r="51" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -2944,8 +2953,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G51" s="41"/>
-      <c r="H51" s="42"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="46"/>
     </row>
     <row r="52" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -2967,8 +2976,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G52" s="41"/>
-      <c r="H52" s="42"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="46"/>
     </row>
     <row r="53" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -2990,8 +2999,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G53" s="41"/>
-      <c r="H53" s="42"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="46"/>
     </row>
     <row r="54" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18">
@@ -3013,11 +3022,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G54" s="41">
+      <c r="G54" s="43">
         <f>SUM(F54:F122)</f>
         <v>321</v>
       </c>
-      <c r="H54" s="42" t="str">
+      <c r="H54" s="46" t="str">
         <f xml:space="preserve"> IF(G54&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -3042,8 +3051,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G55" s="41"/>
-      <c r="H55" s="42"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="46"/>
     </row>
     <row r="56" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18">
@@ -3065,8 +3074,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G56" s="41"/>
-      <c r="H56" s="42"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="46"/>
     </row>
     <row r="57" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
@@ -3088,8 +3097,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G57" s="41"/>
-      <c r="H57" s="42"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="46"/>
     </row>
     <row r="58" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
@@ -3111,8 +3120,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G58" s="41"/>
-      <c r="H58" s="42"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="46"/>
     </row>
     <row r="59" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
@@ -3134,8 +3143,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G59" s="41"/>
-      <c r="H59" s="42"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="46"/>
     </row>
     <row r="60" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
@@ -3157,8 +3166,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G60" s="41"/>
-      <c r="H60" s="42"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="46"/>
     </row>
     <row r="61" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
@@ -3180,8 +3189,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G61" s="41"/>
-      <c r="H61" s="42"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="46"/>
     </row>
     <row r="62" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
@@ -3203,8 +3212,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G62" s="41"/>
-      <c r="H62" s="42"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="46"/>
     </row>
     <row r="63" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
@@ -3226,8 +3235,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G63" s="41"/>
-      <c r="H63" s="42"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="46"/>
     </row>
     <row r="64" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
@@ -3249,8 +3258,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G64" s="41"/>
-      <c r="H64" s="42"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="46"/>
     </row>
     <row r="65" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18">
@@ -3272,8 +3281,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G65" s="41"/>
-      <c r="H65" s="42"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="46"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="18">
@@ -3295,8 +3304,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G66" s="41"/>
-      <c r="H66" s="42"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="46"/>
     </row>
     <row r="67" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A67" s="35">
@@ -3318,8 +3327,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G67" s="41"/>
-      <c r="H67" s="42"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="46"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="35">
@@ -3341,8 +3350,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G68" s="41"/>
-      <c r="H68" s="42"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="46"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="35">
@@ -3364,8 +3373,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G69" s="41"/>
-      <c r="H69" s="42"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="46"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="35">
@@ -3387,8 +3396,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G70" s="41"/>
-      <c r="H70" s="42"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="46"/>
     </row>
     <row r="71" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A71" s="35">
@@ -3410,8 +3419,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G71" s="41"/>
-      <c r="H71" s="42"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="46"/>
     </row>
     <row r="72" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A72" s="35">
@@ -3433,8 +3442,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G72" s="41"/>
-      <c r="H72" s="42"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="46"/>
     </row>
     <row r="73" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A73" s="35">
@@ -3456,8 +3465,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G73" s="41"/>
-      <c r="H73" s="42"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="46"/>
     </row>
     <row r="74" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A74" s="35">
@@ -3479,8 +3488,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G74" s="41"/>
-      <c r="H74" s="42"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="46"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="35">
@@ -3502,8 +3511,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G75" s="41"/>
-      <c r="H75" s="42"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="46"/>
     </row>
     <row r="76" spans="1:8" ht="43.8" x14ac:dyDescent="0.25">
       <c r="A76" s="35">
@@ -3525,8 +3534,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G76" s="41"/>
-      <c r="H76" s="42"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="46"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="35">
@@ -3548,8 +3557,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G77" s="41"/>
-      <c r="H77" s="42"/>
+      <c r="G77" s="43"/>
+      <c r="H77" s="46"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="35">
@@ -3571,8 +3580,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G78" s="41"/>
-      <c r="H78" s="42"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="46"/>
     </row>
     <row r="79" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A79" s="35">
@@ -3594,8 +3603,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G79" s="41"/>
-      <c r="H79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="46"/>
     </row>
     <row r="80" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A80" s="35">
@@ -3617,8 +3626,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G80" s="41"/>
-      <c r="H80" s="42"/>
+      <c r="G80" s="43"/>
+      <c r="H80" s="46"/>
     </row>
     <row r="81" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A81" s="35">
@@ -3640,8 +3649,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G81" s="41"/>
-      <c r="H81" s="42"/>
+      <c r="G81" s="43"/>
+      <c r="H81" s="46"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="35">
@@ -3663,8 +3672,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G82" s="41"/>
-      <c r="H82" s="42"/>
+      <c r="G82" s="43"/>
+      <c r="H82" s="46"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="35">
@@ -3686,8 +3695,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G83" s="41"/>
-      <c r="H83" s="42"/>
+      <c r="G83" s="43"/>
+      <c r="H83" s="46"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="35">
@@ -3709,8 +3718,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G84" s="41"/>
-      <c r="H84" s="42"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="46"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="35">
@@ -3732,8 +3741,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G85" s="41"/>
-      <c r="H85" s="42"/>
+      <c r="G85" s="43"/>
+      <c r="H85" s="46"/>
     </row>
     <row r="86" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A86" s="35">
@@ -3755,8 +3764,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G86" s="41"/>
-      <c r="H86" s="42"/>
+      <c r="G86" s="43"/>
+      <c r="H86" s="46"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="35">
@@ -3778,8 +3787,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G87" s="41"/>
-      <c r="H87" s="42"/>
+      <c r="G87" s="43"/>
+      <c r="H87" s="46"/>
     </row>
     <row r="88" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A88" s="35">
@@ -3801,8 +3810,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G88" s="41"/>
-      <c r="H88" s="42"/>
+      <c r="G88" s="43"/>
+      <c r="H88" s="46"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="35">
@@ -3824,8 +3833,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G89" s="41"/>
-      <c r="H89" s="42"/>
+      <c r="G89" s="43"/>
+      <c r="H89" s="46"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="35">
@@ -3847,8 +3856,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G90" s="41"/>
-      <c r="H90" s="42"/>
+      <c r="G90" s="43"/>
+      <c r="H90" s="46"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="35">
@@ -3870,8 +3879,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G91" s="41"/>
-      <c r="H91" s="42"/>
+      <c r="G91" s="43"/>
+      <c r="H91" s="46"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="35">
@@ -3893,8 +3902,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G92" s="41"/>
-      <c r="H92" s="42"/>
+      <c r="G92" s="43"/>
+      <c r="H92" s="46"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="35">
@@ -3916,8 +3925,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G93" s="41"/>
-      <c r="H93" s="42"/>
+      <c r="G93" s="43"/>
+      <c r="H93" s="46"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="35">
@@ -3939,8 +3948,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G94" s="41"/>
-      <c r="H94" s="42"/>
+      <c r="G94" s="43"/>
+      <c r="H94" s="46"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="35">
@@ -3962,8 +3971,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G95" s="41"/>
-      <c r="H95" s="42"/>
+      <c r="G95" s="43"/>
+      <c r="H95" s="46"/>
     </row>
     <row r="96" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A96" s="35">
@@ -3985,8 +3994,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G96" s="41"/>
-      <c r="H96" s="42"/>
+      <c r="G96" s="43"/>
+      <c r="H96" s="46"/>
     </row>
     <row r="97" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A97" s="35">
@@ -4008,8 +4017,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G97" s="41"/>
-      <c r="H97" s="42"/>
+      <c r="G97" s="43"/>
+      <c r="H97" s="46"/>
     </row>
     <row r="98" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A98" s="35">
@@ -4031,8 +4040,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G98" s="41"/>
-      <c r="H98" s="42"/>
+      <c r="G98" s="43"/>
+      <c r="H98" s="46"/>
     </row>
     <row r="99" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A99" s="35">
@@ -4054,8 +4063,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G99" s="41"/>
-      <c r="H99" s="42"/>
+      <c r="G99" s="43"/>
+      <c r="H99" s="46"/>
     </row>
     <row r="100" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A100" s="35">
@@ -4077,8 +4086,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G100" s="41"/>
-      <c r="H100" s="42"/>
+      <c r="G100" s="43"/>
+      <c r="H100" s="46"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="35">
@@ -4100,8 +4109,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G101" s="41"/>
-      <c r="H101" s="42"/>
+      <c r="G101" s="43"/>
+      <c r="H101" s="46"/>
     </row>
     <row r="102" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A102" s="35">
@@ -4123,8 +4132,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G102" s="41"/>
-      <c r="H102" s="42"/>
+      <c r="G102" s="43"/>
+      <c r="H102" s="46"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="35">
@@ -4146,8 +4155,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G103" s="41"/>
-      <c r="H103" s="42"/>
+      <c r="G103" s="43"/>
+      <c r="H103" s="46"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="35">
@@ -4169,8 +4178,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G104" s="41"/>
-      <c r="H104" s="42"/>
+      <c r="G104" s="43"/>
+      <c r="H104" s="46"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="35">
@@ -4192,8 +4201,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G105" s="41"/>
-      <c r="H105" s="42"/>
+      <c r="G105" s="43"/>
+      <c r="H105" s="46"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="35">
@@ -4215,8 +4224,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G106" s="41"/>
-      <c r="H106" s="42"/>
+      <c r="G106" s="43"/>
+      <c r="H106" s="46"/>
     </row>
     <row r="107" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A107" s="35">
@@ -4238,8 +4247,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G107" s="41"/>
-      <c r="H107" s="42"/>
+      <c r="G107" s="43"/>
+      <c r="H107" s="46"/>
     </row>
     <row r="108" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A108" s="35">
@@ -4261,8 +4270,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G108" s="41"/>
-      <c r="H108" s="42"/>
+      <c r="G108" s="43"/>
+      <c r="H108" s="46"/>
     </row>
     <row r="109" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A109" s="35">
@@ -4284,8 +4293,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G109" s="41"/>
-      <c r="H109" s="42"/>
+      <c r="G109" s="43"/>
+      <c r="H109" s="46"/>
     </row>
     <row r="110" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A110" s="35">
@@ -4307,8 +4316,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G110" s="41"/>
-      <c r="H110" s="42"/>
+      <c r="G110" s="43"/>
+      <c r="H110" s="46"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="35">
@@ -4330,8 +4339,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G111" s="41"/>
-      <c r="H111" s="42"/>
+      <c r="G111" s="43"/>
+      <c r="H111" s="46"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="35">
@@ -4353,8 +4362,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G112" s="41"/>
-      <c r="H112" s="42"/>
+      <c r="G112" s="43"/>
+      <c r="H112" s="46"/>
     </row>
     <row r="113" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A113" s="35">
@@ -4376,8 +4385,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G113" s="41"/>
-      <c r="H113" s="42"/>
+      <c r="G113" s="43"/>
+      <c r="H113" s="46"/>
     </row>
     <row r="114" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A114" s="35">
@@ -4399,8 +4408,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G114" s="41"/>
-      <c r="H114" s="42"/>
+      <c r="G114" s="43"/>
+      <c r="H114" s="46"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="35">
@@ -4422,8 +4431,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G115" s="41"/>
-      <c r="H115" s="42"/>
+      <c r="G115" s="43"/>
+      <c r="H115" s="46"/>
     </row>
     <row r="116" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A116" s="35">
@@ -4445,8 +4454,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G116" s="41"/>
-      <c r="H116" s="42"/>
+      <c r="G116" s="43"/>
+      <c r="H116" s="46"/>
     </row>
     <row r="117" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A117" s="35">
@@ -4468,8 +4477,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G117" s="41"/>
-      <c r="H117" s="42"/>
+      <c r="G117" s="43"/>
+      <c r="H117" s="46"/>
     </row>
     <row r="118" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A118" s="35">
@@ -4491,8 +4500,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G118" s="41"/>
-      <c r="H118" s="42"/>
+      <c r="G118" s="43"/>
+      <c r="H118" s="46"/>
     </row>
     <row r="119" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A119" s="35">
@@ -4514,8 +4523,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G119" s="41"/>
-      <c r="H119" s="42"/>
+      <c r="G119" s="43"/>
+      <c r="H119" s="46"/>
     </row>
     <row r="120" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A120" s="35">
@@ -4537,8 +4546,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G120" s="41"/>
-      <c r="H120" s="42"/>
+      <c r="G120" s="43"/>
+      <c r="H120" s="46"/>
     </row>
     <row r="121" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A121" s="35">
@@ -4560,8 +4569,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G121" s="41"/>
-      <c r="H121" s="42"/>
+      <c r="G121" s="43"/>
+      <c r="H121" s="46"/>
     </row>
     <row r="122" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A122" s="35">
@@ -4583,8 +4592,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G122" s="41"/>
-      <c r="H122" s="42"/>
+      <c r="G122" s="43"/>
+      <c r="H122" s="46"/>
     </row>
     <row r="123" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="35">
@@ -4606,11 +4615,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G123" s="41">
-        <f>SUM(F123:F177)</f>
-        <v>264</v>
-      </c>
-      <c r="H123" s="42" t="str">
+      <c r="G123" s="43">
+        <f>SUM(F123:F178)</f>
+        <v>265</v>
+      </c>
+      <c r="H123" s="46" t="str">
         <f xml:space="preserve"> IF(G123&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -4635,8 +4644,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G124" s="41"/>
-      <c r="H124" s="42"/>
+      <c r="G124" s="43"/>
+      <c r="H124" s="46"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="35">
@@ -4658,8 +4667,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G125" s="41"/>
-      <c r="H125" s="42"/>
+      <c r="G125" s="43"/>
+      <c r="H125" s="46"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="35">
@@ -4681,8 +4690,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G126" s="41"/>
-      <c r="H126" s="42"/>
+      <c r="G126" s="43"/>
+      <c r="H126" s="46"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="35">
@@ -4704,8 +4713,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G127" s="41"/>
-      <c r="H127" s="42"/>
+      <c r="G127" s="43"/>
+      <c r="H127" s="46"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="38">
@@ -4727,8 +4736,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G128" s="41"/>
-      <c r="H128" s="42"/>
+      <c r="G128" s="43"/>
+      <c r="H128" s="46"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="38">
@@ -4750,8 +4759,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G129" s="41"/>
-      <c r="H129" s="42"/>
+      <c r="G129" s="43"/>
+      <c r="H129" s="46"/>
     </row>
     <row r="130" spans="1:9" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A130" s="38">
@@ -4773,8 +4782,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G130" s="41"/>
-      <c r="H130" s="42"/>
+      <c r="G130" s="43"/>
+      <c r="H130" s="46"/>
     </row>
     <row r="131" spans="1:9" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A131" s="38">
@@ -4796,8 +4805,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G131" s="41"/>
-      <c r="H131" s="42"/>
+      <c r="G131" s="43"/>
+      <c r="H131" s="46"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="38">
@@ -4819,8 +4828,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G132" s="41"/>
-      <c r="H132" s="42"/>
+      <c r="G132" s="43"/>
+      <c r="H132" s="46"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="38">
@@ -4842,8 +4851,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G133" s="41"/>
-      <c r="H133" s="42"/>
+      <c r="G133" s="43"/>
+      <c r="H133" s="46"/>
     </row>
     <row r="134" spans="1:9" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A134" s="38">
@@ -4865,8 +4874,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G134" s="41"/>
-      <c r="H134" s="42"/>
+      <c r="G134" s="43"/>
+      <c r="H134" s="46"/>
       <c r="I134" s="22"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -4889,8 +4898,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G135" s="41"/>
-      <c r="H135" s="42"/>
+      <c r="G135" s="43"/>
+      <c r="H135" s="46"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="38">
@@ -4912,8 +4921,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G136" s="41"/>
-      <c r="H136" s="42"/>
+      <c r="G136" s="43"/>
+      <c r="H136" s="46"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="38">
@@ -4935,8 +4944,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G137" s="41"/>
-      <c r="H137" s="42"/>
+      <c r="G137" s="43"/>
+      <c r="H137" s="46"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="38">
@@ -4958,8 +4967,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G138" s="41"/>
-      <c r="H138" s="42"/>
+      <c r="G138" s="43"/>
+      <c r="H138" s="46"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="38">
@@ -4981,8 +4990,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G139" s="41"/>
-      <c r="H139" s="42"/>
+      <c r="G139" s="43"/>
+      <c r="H139" s="46"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="38">
@@ -5004,8 +5013,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G140" s="41"/>
-      <c r="H140" s="42"/>
+      <c r="G140" s="43"/>
+      <c r="H140" s="46"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="38">
@@ -5027,8 +5036,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G141" s="41"/>
-      <c r="H141" s="42"/>
+      <c r="G141" s="43"/>
+      <c r="H141" s="46"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="38">
@@ -5050,8 +5059,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G142" s="41"/>
-      <c r="H142" s="42"/>
+      <c r="G142" s="43"/>
+      <c r="H142" s="46"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="38">
@@ -5073,8 +5082,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G143" s="41"/>
-      <c r="H143" s="42"/>
+      <c r="G143" s="43"/>
+      <c r="H143" s="46"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="38">
@@ -5096,8 +5105,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G144" s="41"/>
-      <c r="H144" s="42"/>
+      <c r="G144" s="43"/>
+      <c r="H144" s="46"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="38">
@@ -5119,8 +5128,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G145" s="41"/>
-      <c r="H145" s="42"/>
+      <c r="G145" s="43"/>
+      <c r="H145" s="46"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="38">
@@ -5142,8 +5151,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G146" s="41"/>
-      <c r="H146" s="42"/>
+      <c r="G146" s="43"/>
+      <c r="H146" s="46"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="38">
@@ -5165,8 +5174,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G147" s="41"/>
-      <c r="H147" s="42"/>
+      <c r="G147" s="43"/>
+      <c r="H147" s="46"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="38">
@@ -5188,8 +5197,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G148" s="41"/>
-      <c r="H148" s="42"/>
+      <c r="G148" s="43"/>
+      <c r="H148" s="46"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="38">
@@ -5211,8 +5220,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G149" s="41"/>
-      <c r="H149" s="42"/>
+      <c r="G149" s="43"/>
+      <c r="H149" s="46"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="38">
@@ -5234,8 +5243,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G150" s="41"/>
-      <c r="H150" s="42"/>
+      <c r="G150" s="43"/>
+      <c r="H150" s="46"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="38">
@@ -5257,8 +5266,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G151" s="41"/>
-      <c r="H151" s="42"/>
+      <c r="G151" s="43"/>
+      <c r="H151" s="46"/>
     </row>
     <row r="152" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A152" s="38">
@@ -5280,8 +5289,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G152" s="41"/>
-      <c r="H152" s="42"/>
+      <c r="G152" s="43"/>
+      <c r="H152" s="46"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="38">
@@ -5303,8 +5312,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G153" s="41"/>
-      <c r="H153" s="42"/>
+      <c r="G153" s="43"/>
+      <c r="H153" s="46"/>
     </row>
     <row r="154" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A154" s="38">
@@ -5326,8 +5335,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G154" s="41"/>
-      <c r="H154" s="42"/>
+      <c r="G154" s="43"/>
+      <c r="H154" s="46"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="38">
@@ -5349,8 +5358,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G155" s="41"/>
-      <c r="H155" s="42"/>
+      <c r="G155" s="43"/>
+      <c r="H155" s="46"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="38">
@@ -5372,8 +5381,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G156" s="41"/>
-      <c r="H156" s="42"/>
+      <c r="G156" s="43"/>
+      <c r="H156" s="46"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="38">
@@ -5395,8 +5404,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G157" s="41"/>
-      <c r="H157" s="42"/>
+      <c r="G157" s="43"/>
+      <c r="H157" s="46"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="38">
@@ -5418,8 +5427,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G158" s="41"/>
-      <c r="H158" s="42"/>
+      <c r="G158" s="43"/>
+      <c r="H158" s="46"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="38">
@@ -5441,8 +5450,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G159" s="41"/>
-      <c r="H159" s="42"/>
+      <c r="G159" s="43"/>
+      <c r="H159" s="46"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="38">
@@ -5464,8 +5473,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G160" s="41"/>
-      <c r="H160" s="42"/>
+      <c r="G160" s="43"/>
+      <c r="H160" s="46"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="38">
@@ -5487,8 +5496,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G161" s="41"/>
-      <c r="H161" s="42"/>
+      <c r="G161" s="43"/>
+      <c r="H161" s="46"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="38">
@@ -5510,8 +5519,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G162" s="41"/>
-      <c r="H162" s="42"/>
+      <c r="G162" s="43"/>
+      <c r="H162" s="46"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="38">
@@ -5533,8 +5542,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G163" s="41"/>
-      <c r="H163" s="42"/>
+      <c r="G163" s="43"/>
+      <c r="H163" s="46"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="38">
@@ -5556,8 +5565,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G164" s="41"/>
-      <c r="H164" s="42"/>
+      <c r="G164" s="43"/>
+      <c r="H164" s="46"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="38">
@@ -5579,8 +5588,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G165" s="41"/>
-      <c r="H165" s="42"/>
+      <c r="G165" s="43"/>
+      <c r="H165" s="46"/>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="38">
@@ -5602,8 +5611,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G166" s="41"/>
-      <c r="H166" s="42"/>
+      <c r="G166" s="43"/>
+      <c r="H166" s="46"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="38">
@@ -5625,8 +5634,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G167" s="41"/>
-      <c r="H167" s="42"/>
+      <c r="G167" s="43"/>
+      <c r="H167" s="46"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="38">
@@ -5648,8 +5657,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G168" s="41"/>
-      <c r="H168" s="42"/>
+      <c r="G168" s="43"/>
+      <c r="H168" s="46"/>
     </row>
     <row r="169" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A169" s="38">
@@ -5671,8 +5680,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G169" s="41"/>
-      <c r="H169" s="42"/>
+      <c r="G169" s="43"/>
+      <c r="H169" s="46"/>
     </row>
     <row r="170" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A170" s="38">
@@ -5694,8 +5703,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G170" s="41"/>
-      <c r="H170" s="42"/>
+      <c r="G170" s="43"/>
+      <c r="H170" s="46"/>
     </row>
     <row r="171" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A171" s="38">
@@ -5717,8 +5726,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G171" s="41"/>
-      <c r="H171" s="42"/>
+      <c r="G171" s="43"/>
+      <c r="H171" s="46"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="38">
@@ -5740,8 +5749,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G172" s="41"/>
-      <c r="H172" s="42"/>
+      <c r="G172" s="43"/>
+      <c r="H172" s="46"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="38">
@@ -5763,8 +5772,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G173" s="41"/>
-      <c r="H173" s="42"/>
+      <c r="G173" s="43"/>
+      <c r="H173" s="46"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="38">
@@ -5786,8 +5795,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G174" s="41"/>
-      <c r="H174" s="42"/>
+      <c r="G174" s="43"/>
+      <c r="H174" s="46"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="38">
@@ -5809,8 +5818,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G175" s="41"/>
-      <c r="H175" s="42"/>
+      <c r="G175" s="43"/>
+      <c r="H175" s="46"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="38">
@@ -5832,8 +5841,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G176" s="41"/>
-      <c r="H176" s="42"/>
+      <c r="G176" s="43"/>
+      <c r="H176" s="46"/>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="38">
@@ -5855,22 +5864,31 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G177" s="41"/>
-      <c r="H177" s="22"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G177" s="43"/>
+      <c r="H177" s="46"/>
+    </row>
+    <row r="178" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
       <c r="A178" s="38">
         <v>176</v>
       </c>
       <c r="B178" s="23">
         <v>5</v>
       </c>
-      <c r="E178" s="18"/>
-      <c r="F178" s="18" t="str">
+      <c r="C178" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="D178" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="E178" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F178" s="18">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H178" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="G178" s="43"/>
+      <c r="H178" s="46"/>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="38">
@@ -9332,15 +9350,15 @@
   <mergeCells count="11">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="H3:H7"/>
-    <mergeCell ref="G123:G177"/>
     <mergeCell ref="G3:G7"/>
-    <mergeCell ref="H123:H176"/>
     <mergeCell ref="G8:G32"/>
     <mergeCell ref="H8:H32"/>
     <mergeCell ref="G33:G53"/>
     <mergeCell ref="H33:H53"/>
     <mergeCell ref="G54:G122"/>
     <mergeCell ref="H54:H122"/>
+    <mergeCell ref="G123:G178"/>
+    <mergeCell ref="H123:H178"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2 H33 H54 C138 C144 C161 C167 C169 H192:H1048576 H123">
     <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Stop current Development">
@@ -9383,8 +9401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B167" workbookViewId="0">
-      <selection activeCell="H177" sqref="H177"/>
+    <sheetView topLeftCell="B167" workbookViewId="0">
+      <selection activeCell="C176" sqref="C176:D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -14253,8 +14271,14 @@
         <f>'Bug Metrics'!$B182</f>
         <v>5</v>
       </c>
-      <c r="C177" s="9"/>
-      <c r="D177" s="10"/>
+      <c r="C177" s="9" t="str">
+        <f>'Bug Metrics'!$C178</f>
+        <v>Index</v>
+      </c>
+      <c r="D177" s="10" t="str">
+        <f>'Bug Metrics'!$D178</f>
+        <v>Information about round number, status and student edollar balance is repeated on home page</v>
+      </c>
       <c r="E177" s="11"/>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>

</xml_diff>

<commit_message>
tested web service and debugged dump.php
Co-Authored-By: j1em1n <j1em1n@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\GitHub\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2167CA-DDB2-443C-8D91-1713EE09CD3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCC0862-7D24-4E51-BA54-63CEEC655B7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="237">
   <si>
     <t>Bug Log</t>
   </si>
@@ -741,6 +741,9 @@
   </si>
   <si>
     <t>Information about round number, status and student edollar balance is repeated on home page</t>
+  </si>
+  <si>
+    <t>Test case 185-dump - section-student is populated with ALL successful bids across round 1 and round 2, should only should previous round</t>
   </si>
 </sst>
 </file>
@@ -1109,6 +1112,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1121,16 +1127,10 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1142,18 +1142,42 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1186,27 +1210,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFABDFDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1772,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="72" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123:G178"/>
+    <sheetView topLeftCell="A172" zoomScale="72" workbookViewId="0">
+      <selection activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.6" x14ac:dyDescent="0.25"/>
@@ -1791,16 +1794,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -1851,7 +1854,7 @@
         <f>SUM(F3:F7)</f>
         <v>26</v>
       </c>
-      <c r="H3" s="40" t="str">
+      <c r="H3" s="41" t="str">
         <f xml:space="preserve"> IF(G3&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1876,7 +1879,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="45"/>
-      <c r="H4" s="41"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
@@ -1898,7 +1901,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="45"/>
-      <c r="H5" s="41"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
@@ -1920,7 +1923,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="45"/>
-      <c r="H6" s="41"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="7" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
@@ -1942,7 +1945,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="45"/>
-      <c r="H7" s="42"/>
+      <c r="H7" s="43"/>
     </row>
     <row r="8" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="25">
@@ -1963,11 +1966,11 @@
       <c r="F8" s="25">
         <v>5</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="46">
         <f>SUM(F8:F32)</f>
         <v>156</v>
       </c>
-      <c r="H8" s="48" t="str">
+      <c r="H8" s="47" t="str">
         <f xml:space="preserve"> IF(G8&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -1991,8 +1994,8 @@
       <c r="F9" s="25">
         <v>5</v>
       </c>
-      <c r="G9" s="47"/>
-      <c r="H9" s="49"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="25">
@@ -2013,8 +2016,8 @@
       <c r="F10" s="25">
         <v>5</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="49"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:8" ht="44.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="25">
@@ -2035,8 +2038,8 @@
       <c r="F11" s="25">
         <v>10</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="49"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="48"/>
     </row>
     <row r="12" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25">
@@ -2057,8 +2060,8 @@
       <c r="F12" s="25">
         <v>10</v>
       </c>
-      <c r="G12" s="47"/>
-      <c r="H12" s="49"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="25">
@@ -2079,8 +2082,8 @@
       <c r="F13" s="25">
         <v>10</v>
       </c>
-      <c r="G13" s="47"/>
-      <c r="H13" s="49"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25">
@@ -2101,8 +2104,8 @@
       <c r="F14" s="25">
         <v>10</v>
       </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="49"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="25">
@@ -2123,8 +2126,8 @@
       <c r="F15" s="25">
         <v>10</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="49"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="29">
@@ -2145,8 +2148,8 @@
       <c r="F16" s="25">
         <v>5</v>
       </c>
-      <c r="G16" s="47"/>
-      <c r="H16" s="49"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="48"/>
     </row>
     <row r="17" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="30">
@@ -2167,8 +2170,8 @@
       <c r="F17" s="25">
         <v>1</v>
       </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="49"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="48"/>
     </row>
     <row r="18" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="30">
@@ -2189,8 +2192,8 @@
       <c r="F18" s="25">
         <v>5</v>
       </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="49"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="48"/>
     </row>
     <row r="19" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="31">
@@ -2211,8 +2214,8 @@
       <c r="F19" s="25">
         <v>1</v>
       </c>
-      <c r="G19" s="47"/>
-      <c r="H19" s="49"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="18">
@@ -2234,8 +2237,8 @@
         <f t="shared" ref="F20:F187" si="0">IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="G20" s="47"/>
-      <c r="H20" s="49"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="48"/>
     </row>
     <row r="21" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="18">
@@ -2257,8 +2260,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G21" s="47"/>
-      <c r="H21" s="49"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18">
@@ -2280,8 +2283,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G22" s="47"/>
-      <c r="H22" s="49"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="18">
@@ -2303,8 +2306,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G23" s="47"/>
-      <c r="H23" s="49"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="18">
@@ -2326,8 +2329,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G24" s="47"/>
-      <c r="H24" s="49"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="18">
@@ -2349,8 +2352,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G25" s="47"/>
-      <c r="H25" s="49"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="18">
@@ -2372,8 +2375,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G26" s="47"/>
-      <c r="H26" s="49"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="48"/>
     </row>
     <row r="27" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="18">
@@ -2395,8 +2398,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G27" s="47"/>
-      <c r="H27" s="49"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="48"/>
     </row>
     <row r="28" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="18">
@@ -2418,8 +2421,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G28" s="47"/>
-      <c r="H28" s="49"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18">
@@ -2441,8 +2444,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G29" s="47"/>
-      <c r="H29" s="49"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="48"/>
     </row>
     <row r="30" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="18">
@@ -2464,8 +2467,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="49"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="48"/>
     </row>
     <row r="31" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="18">
@@ -2487,8 +2490,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G31" s="47"/>
-      <c r="H31" s="49"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="48"/>
     </row>
     <row r="32" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="18">
@@ -2510,8 +2513,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="49"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="48"/>
     </row>
     <row r="33" spans="1:8" ht="15.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
@@ -2533,11 +2536,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G33" s="43">
+      <c r="G33" s="49">
         <f>SUM(F33:F53)</f>
         <v>142</v>
       </c>
-      <c r="H33" s="46" t="str">
+      <c r="H33" s="50" t="str">
         <f xml:space="preserve"> IF(G33&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -2562,8 +2565,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G34" s="43"/>
-      <c r="H34" s="46"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="50"/>
     </row>
     <row r="35" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
@@ -2585,8 +2588,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G35" s="43"/>
-      <c r="H35" s="46"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="50"/>
     </row>
     <row r="36" spans="1:8" ht="23.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18">
@@ -2608,8 +2611,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G36" s="43"/>
-      <c r="H36" s="46"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="50"/>
     </row>
     <row r="37" spans="1:8" ht="23.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18">
@@ -2631,8 +2634,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="46"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="50"/>
     </row>
     <row r="38" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
@@ -2654,8 +2657,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="46"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="50"/>
     </row>
     <row r="39" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18">
@@ -2677,8 +2680,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="46"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="50"/>
     </row>
     <row r="40" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
@@ -2700,8 +2703,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G40" s="43"/>
-      <c r="H40" s="46"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="50"/>
     </row>
     <row r="41" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18">
@@ -2723,8 +2726,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G41" s="43"/>
-      <c r="H41" s="46"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="50"/>
     </row>
     <row r="42" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
@@ -2746,8 +2749,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G42" s="43"/>
-      <c r="H42" s="46"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="50"/>
     </row>
     <row r="43" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
@@ -2769,8 +2772,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="46"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="50"/>
     </row>
     <row r="44" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18">
@@ -2792,8 +2795,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G44" s="43"/>
-      <c r="H44" s="46"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="50"/>
     </row>
     <row r="45" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18">
@@ -2815,8 +2818,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G45" s="43"/>
-      <c r="H45" s="46"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="50"/>
     </row>
     <row r="46" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18">
@@ -2838,8 +2841,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G46" s="43"/>
-      <c r="H46" s="46"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="50"/>
     </row>
     <row r="47" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
@@ -2861,8 +2864,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G47" s="43"/>
-      <c r="H47" s="46"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="50"/>
     </row>
     <row r="48" spans="1:8" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
@@ -2884,8 +2887,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G48" s="43"/>
-      <c r="H48" s="46"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="50"/>
     </row>
     <row r="49" spans="1:8" ht="15.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
@@ -2907,8 +2910,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G49" s="43"/>
-      <c r="H49" s="46"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="50"/>
     </row>
     <row r="50" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
@@ -2930,8 +2933,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G50" s="43"/>
-      <c r="H50" s="46"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="50"/>
     </row>
     <row r="51" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
@@ -2953,8 +2956,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G51" s="43"/>
-      <c r="H51" s="46"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="50"/>
     </row>
     <row r="52" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
@@ -2976,8 +2979,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G52" s="43"/>
-      <c r="H52" s="46"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="50"/>
     </row>
     <row r="53" spans="1:8" ht="29.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
@@ -2999,8 +3002,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G53" s="43"/>
-      <c r="H53" s="46"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="50"/>
     </row>
     <row r="54" spans="1:8" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18">
@@ -3022,11 +3025,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G54" s="43">
+      <c r="G54" s="49">
         <f>SUM(F54:F122)</f>
         <v>321</v>
       </c>
-      <c r="H54" s="46" t="str">
+      <c r="H54" s="50" t="str">
         <f xml:space="preserve"> IF(G54&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -3051,8 +3054,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G55" s="43"/>
-      <c r="H55" s="46"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="50"/>
     </row>
     <row r="56" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18">
@@ -3074,8 +3077,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G56" s="43"/>
-      <c r="H56" s="46"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="50"/>
     </row>
     <row r="57" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
@@ -3097,8 +3100,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G57" s="43"/>
-      <c r="H57" s="46"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="50"/>
     </row>
     <row r="58" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
@@ -3120,8 +3123,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G58" s="43"/>
-      <c r="H58" s="46"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="50"/>
     </row>
     <row r="59" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
@@ -3143,8 +3146,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G59" s="43"/>
-      <c r="H59" s="46"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="50"/>
     </row>
     <row r="60" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
@@ -3166,8 +3169,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G60" s="43"/>
-      <c r="H60" s="46"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="50"/>
     </row>
     <row r="61" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
@@ -3189,8 +3192,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G61" s="43"/>
-      <c r="H61" s="46"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="50"/>
     </row>
     <row r="62" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
@@ -3212,8 +3215,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G62" s="43"/>
-      <c r="H62" s="46"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="50"/>
     </row>
     <row r="63" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
@@ -3235,8 +3238,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G63" s="43"/>
-      <c r="H63" s="46"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="50"/>
     </row>
     <row r="64" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
@@ -3258,8 +3261,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G64" s="43"/>
-      <c r="H64" s="46"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="50"/>
     </row>
     <row r="65" spans="1:8" ht="29.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18">
@@ -3281,8 +3284,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G65" s="43"/>
-      <c r="H65" s="46"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="50"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="18">
@@ -3304,8 +3307,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G66" s="43"/>
-      <c r="H66" s="46"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="50"/>
     </row>
     <row r="67" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A67" s="35">
@@ -3327,8 +3330,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G67" s="43"/>
-      <c r="H67" s="46"/>
+      <c r="G67" s="49"/>
+      <c r="H67" s="50"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="35">
@@ -3350,8 +3353,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G68" s="43"/>
-      <c r="H68" s="46"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="50"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="35">
@@ -3373,8 +3376,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G69" s="43"/>
-      <c r="H69" s="46"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="35">
@@ -3396,8 +3399,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G70" s="43"/>
-      <c r="H70" s="46"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="50"/>
     </row>
     <row r="71" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A71" s="35">
@@ -3419,8 +3422,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G71" s="43"/>
-      <c r="H71" s="46"/>
+      <c r="G71" s="49"/>
+      <c r="H71" s="50"/>
     </row>
     <row r="72" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A72" s="35">
@@ -3442,8 +3445,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G72" s="43"/>
-      <c r="H72" s="46"/>
+      <c r="G72" s="49"/>
+      <c r="H72" s="50"/>
     </row>
     <row r="73" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A73" s="35">
@@ -3465,8 +3468,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G73" s="43"/>
-      <c r="H73" s="46"/>
+      <c r="G73" s="49"/>
+      <c r="H73" s="50"/>
     </row>
     <row r="74" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A74" s="35">
@@ -3488,8 +3491,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G74" s="43"/>
-      <c r="H74" s="46"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="50"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="35">
@@ -3511,8 +3514,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G75" s="43"/>
-      <c r="H75" s="46"/>
+      <c r="G75" s="49"/>
+      <c r="H75" s="50"/>
     </row>
     <row r="76" spans="1:8" ht="43.8" x14ac:dyDescent="0.25">
       <c r="A76" s="35">
@@ -3534,8 +3537,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G76" s="43"/>
-      <c r="H76" s="46"/>
+      <c r="G76" s="49"/>
+      <c r="H76" s="50"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="35">
@@ -3557,8 +3560,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G77" s="43"/>
-      <c r="H77" s="46"/>
+      <c r="G77" s="49"/>
+      <c r="H77" s="50"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="35">
@@ -3580,8 +3583,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G78" s="43"/>
-      <c r="H78" s="46"/>
+      <c r="G78" s="49"/>
+      <c r="H78" s="50"/>
     </row>
     <row r="79" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A79" s="35">
@@ -3603,8 +3606,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G79" s="43"/>
-      <c r="H79" s="46"/>
+      <c r="G79" s="49"/>
+      <c r="H79" s="50"/>
     </row>
     <row r="80" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A80" s="35">
@@ -3626,8 +3629,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G80" s="43"/>
-      <c r="H80" s="46"/>
+      <c r="G80" s="49"/>
+      <c r="H80" s="50"/>
     </row>
     <row r="81" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A81" s="35">
@@ -3649,8 +3652,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G81" s="43"/>
-      <c r="H81" s="46"/>
+      <c r="G81" s="49"/>
+      <c r="H81" s="50"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="35">
@@ -3672,8 +3675,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G82" s="43"/>
-      <c r="H82" s="46"/>
+      <c r="G82" s="49"/>
+      <c r="H82" s="50"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="35">
@@ -3695,8 +3698,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G83" s="43"/>
-      <c r="H83" s="46"/>
+      <c r="G83" s="49"/>
+      <c r="H83" s="50"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="35">
@@ -3718,8 +3721,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G84" s="43"/>
-      <c r="H84" s="46"/>
+      <c r="G84" s="49"/>
+      <c r="H84" s="50"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="35">
@@ -3741,8 +3744,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G85" s="43"/>
-      <c r="H85" s="46"/>
+      <c r="G85" s="49"/>
+      <c r="H85" s="50"/>
     </row>
     <row r="86" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A86" s="35">
@@ -3764,8 +3767,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G86" s="43"/>
-      <c r="H86" s="46"/>
+      <c r="G86" s="49"/>
+      <c r="H86" s="50"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="35">
@@ -3787,8 +3790,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G87" s="43"/>
-      <c r="H87" s="46"/>
+      <c r="G87" s="49"/>
+      <c r="H87" s="50"/>
     </row>
     <row r="88" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A88" s="35">
@@ -3810,8 +3813,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G88" s="43"/>
-      <c r="H88" s="46"/>
+      <c r="G88" s="49"/>
+      <c r="H88" s="50"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="35">
@@ -3833,8 +3836,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G89" s="43"/>
-      <c r="H89" s="46"/>
+      <c r="G89" s="49"/>
+      <c r="H89" s="50"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="35">
@@ -3856,8 +3859,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G90" s="43"/>
-      <c r="H90" s="46"/>
+      <c r="G90" s="49"/>
+      <c r="H90" s="50"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="35">
@@ -3879,8 +3882,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G91" s="43"/>
-      <c r="H91" s="46"/>
+      <c r="G91" s="49"/>
+      <c r="H91" s="50"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="35">
@@ -3902,8 +3905,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G92" s="43"/>
-      <c r="H92" s="46"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="50"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="35">
@@ -3925,8 +3928,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G93" s="43"/>
-      <c r="H93" s="46"/>
+      <c r="G93" s="49"/>
+      <c r="H93" s="50"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="35">
@@ -3948,8 +3951,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G94" s="43"/>
-      <c r="H94" s="46"/>
+      <c r="G94" s="49"/>
+      <c r="H94" s="50"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="35">
@@ -3971,8 +3974,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G95" s="43"/>
-      <c r="H95" s="46"/>
+      <c r="G95" s="49"/>
+      <c r="H95" s="50"/>
     </row>
     <row r="96" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A96" s="35">
@@ -3994,8 +3997,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G96" s="43"/>
-      <c r="H96" s="46"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="50"/>
     </row>
     <row r="97" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A97" s="35">
@@ -4017,8 +4020,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G97" s="43"/>
-      <c r="H97" s="46"/>
+      <c r="G97" s="49"/>
+      <c r="H97" s="50"/>
     </row>
     <row r="98" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A98" s="35">
@@ -4040,8 +4043,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G98" s="43"/>
-      <c r="H98" s="46"/>
+      <c r="G98" s="49"/>
+      <c r="H98" s="50"/>
     </row>
     <row r="99" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A99" s="35">
@@ -4063,8 +4066,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G99" s="43"/>
-      <c r="H99" s="46"/>
+      <c r="G99" s="49"/>
+      <c r="H99" s="50"/>
     </row>
     <row r="100" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A100" s="35">
@@ -4086,8 +4089,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G100" s="43"/>
-      <c r="H100" s="46"/>
+      <c r="G100" s="49"/>
+      <c r="H100" s="50"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="35">
@@ -4109,8 +4112,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G101" s="43"/>
-      <c r="H101" s="46"/>
+      <c r="G101" s="49"/>
+      <c r="H101" s="50"/>
     </row>
     <row r="102" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A102" s="35">
@@ -4132,8 +4135,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G102" s="43"/>
-      <c r="H102" s="46"/>
+      <c r="G102" s="49"/>
+      <c r="H102" s="50"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="35">
@@ -4155,8 +4158,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G103" s="43"/>
-      <c r="H103" s="46"/>
+      <c r="G103" s="49"/>
+      <c r="H103" s="50"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="35">
@@ -4178,8 +4181,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G104" s="43"/>
-      <c r="H104" s="46"/>
+      <c r="G104" s="49"/>
+      <c r="H104" s="50"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="35">
@@ -4201,8 +4204,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G105" s="43"/>
-      <c r="H105" s="46"/>
+      <c r="G105" s="49"/>
+      <c r="H105" s="50"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="35">
@@ -4224,8 +4227,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G106" s="43"/>
-      <c r="H106" s="46"/>
+      <c r="G106" s="49"/>
+      <c r="H106" s="50"/>
     </row>
     <row r="107" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A107" s="35">
@@ -4247,8 +4250,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G107" s="43"/>
-      <c r="H107" s="46"/>
+      <c r="G107" s="49"/>
+      <c r="H107" s="50"/>
     </row>
     <row r="108" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A108" s="35">
@@ -4270,8 +4273,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G108" s="43"/>
-      <c r="H108" s="46"/>
+      <c r="G108" s="49"/>
+      <c r="H108" s="50"/>
     </row>
     <row r="109" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A109" s="35">
@@ -4293,8 +4296,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G109" s="43"/>
-      <c r="H109" s="46"/>
+      <c r="G109" s="49"/>
+      <c r="H109" s="50"/>
     </row>
     <row r="110" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A110" s="35">
@@ -4316,8 +4319,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G110" s="43"/>
-      <c r="H110" s="46"/>
+      <c r="G110" s="49"/>
+      <c r="H110" s="50"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="35">
@@ -4339,8 +4342,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G111" s="43"/>
-      <c r="H111" s="46"/>
+      <c r="G111" s="49"/>
+      <c r="H111" s="50"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="35">
@@ -4362,8 +4365,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G112" s="43"/>
-      <c r="H112" s="46"/>
+      <c r="G112" s="49"/>
+      <c r="H112" s="50"/>
     </row>
     <row r="113" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A113" s="35">
@@ -4385,8 +4388,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G113" s="43"/>
-      <c r="H113" s="46"/>
+      <c r="G113" s="49"/>
+      <c r="H113" s="50"/>
     </row>
     <row r="114" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A114" s="35">
@@ -4408,8 +4411,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G114" s="43"/>
-      <c r="H114" s="46"/>
+      <c r="G114" s="49"/>
+      <c r="H114" s="50"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="35">
@@ -4431,8 +4434,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G115" s="43"/>
-      <c r="H115" s="46"/>
+      <c r="G115" s="49"/>
+      <c r="H115" s="50"/>
     </row>
     <row r="116" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A116" s="35">
@@ -4454,8 +4457,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G116" s="43"/>
-      <c r="H116" s="46"/>
+      <c r="G116" s="49"/>
+      <c r="H116" s="50"/>
     </row>
     <row r="117" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A117" s="35">
@@ -4477,8 +4480,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G117" s="43"/>
-      <c r="H117" s="46"/>
+      <c r="G117" s="49"/>
+      <c r="H117" s="50"/>
     </row>
     <row r="118" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A118" s="35">
@@ -4500,8 +4503,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G118" s="43"/>
-      <c r="H118" s="46"/>
+      <c r="G118" s="49"/>
+      <c r="H118" s="50"/>
     </row>
     <row r="119" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A119" s="35">
@@ -4523,8 +4526,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G119" s="43"/>
-      <c r="H119" s="46"/>
+      <c r="G119" s="49"/>
+      <c r="H119" s="50"/>
     </row>
     <row r="120" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A120" s="35">
@@ -4546,8 +4549,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G120" s="43"/>
-      <c r="H120" s="46"/>
+      <c r="G120" s="49"/>
+      <c r="H120" s="50"/>
     </row>
     <row r="121" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A121" s="35">
@@ -4569,8 +4572,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G121" s="43"/>
-      <c r="H121" s="46"/>
+      <c r="G121" s="49"/>
+      <c r="H121" s="50"/>
     </row>
     <row r="122" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A122" s="35">
@@ -4592,8 +4595,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G122" s="43"/>
-      <c r="H122" s="46"/>
+      <c r="G122" s="49"/>
+      <c r="H122" s="50"/>
     </row>
     <row r="123" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="35">
@@ -4615,11 +4618,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G123" s="43">
+      <c r="G123" s="49">
         <f>SUM(F123:F178)</f>
         <v>265</v>
       </c>
-      <c r="H123" s="46" t="str">
+      <c r="H123" s="50" t="str">
         <f xml:space="preserve"> IF(G123&lt;10,Instructions!$B$7,Instructions!$B$8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
@@ -4644,8 +4647,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G124" s="43"/>
-      <c r="H124" s="46"/>
+      <c r="G124" s="49"/>
+      <c r="H124" s="50"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="35">
@@ -4667,8 +4670,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G125" s="43"/>
-      <c r="H125" s="46"/>
+      <c r="G125" s="49"/>
+      <c r="H125" s="50"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="35">
@@ -4690,8 +4693,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G126" s="43"/>
-      <c r="H126" s="46"/>
+      <c r="G126" s="49"/>
+      <c r="H126" s="50"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="35">
@@ -4713,8 +4716,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G127" s="43"/>
-      <c r="H127" s="46"/>
+      <c r="G127" s="49"/>
+      <c r="H127" s="50"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="38">
@@ -4736,8 +4739,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G128" s="43"/>
-      <c r="H128" s="46"/>
+      <c r="G128" s="49"/>
+      <c r="H128" s="50"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="38">
@@ -4759,8 +4762,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G129" s="43"/>
-      <c r="H129" s="46"/>
+      <c r="G129" s="49"/>
+      <c r="H129" s="50"/>
     </row>
     <row r="130" spans="1:9" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A130" s="38">
@@ -4782,8 +4785,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G130" s="43"/>
-      <c r="H130" s="46"/>
+      <c r="G130" s="49"/>
+      <c r="H130" s="50"/>
     </row>
     <row r="131" spans="1:9" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A131" s="38">
@@ -4805,8 +4808,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G131" s="43"/>
-      <c r="H131" s="46"/>
+      <c r="G131" s="49"/>
+      <c r="H131" s="50"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="38">
@@ -4828,8 +4831,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G132" s="43"/>
-      <c r="H132" s="46"/>
+      <c r="G132" s="49"/>
+      <c r="H132" s="50"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="38">
@@ -4851,8 +4854,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G133" s="43"/>
-      <c r="H133" s="46"/>
+      <c r="G133" s="49"/>
+      <c r="H133" s="50"/>
     </row>
     <row r="134" spans="1:9" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A134" s="38">
@@ -4874,8 +4877,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G134" s="43"/>
-      <c r="H134" s="46"/>
+      <c r="G134" s="49"/>
+      <c r="H134" s="50"/>
       <c r="I134" s="22"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -4898,8 +4901,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G135" s="43"/>
-      <c r="H135" s="46"/>
+      <c r="G135" s="49"/>
+      <c r="H135" s="50"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="38">
@@ -4921,8 +4924,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G136" s="43"/>
-      <c r="H136" s="46"/>
+      <c r="G136" s="49"/>
+      <c r="H136" s="50"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="38">
@@ -4944,8 +4947,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G137" s="43"/>
-      <c r="H137" s="46"/>
+      <c r="G137" s="49"/>
+      <c r="H137" s="50"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="38">
@@ -4967,8 +4970,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G138" s="43"/>
-      <c r="H138" s="46"/>
+      <c r="G138" s="49"/>
+      <c r="H138" s="50"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="38">
@@ -4990,8 +4993,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G139" s="43"/>
-      <c r="H139" s="46"/>
+      <c r="G139" s="49"/>
+      <c r="H139" s="50"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="38">
@@ -5013,8 +5016,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G140" s="43"/>
-      <c r="H140" s="46"/>
+      <c r="G140" s="49"/>
+      <c r="H140" s="50"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="38">
@@ -5036,8 +5039,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G141" s="43"/>
-      <c r="H141" s="46"/>
+      <c r="G141" s="49"/>
+      <c r="H141" s="50"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="38">
@@ -5059,8 +5062,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G142" s="43"/>
-      <c r="H142" s="46"/>
+      <c r="G142" s="49"/>
+      <c r="H142" s="50"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="38">
@@ -5082,8 +5085,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G143" s="43"/>
-      <c r="H143" s="46"/>
+      <c r="G143" s="49"/>
+      <c r="H143" s="50"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="38">
@@ -5105,8 +5108,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G144" s="43"/>
-      <c r="H144" s="46"/>
+      <c r="G144" s="49"/>
+      <c r="H144" s="50"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="38">
@@ -5128,8 +5131,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G145" s="43"/>
-      <c r="H145" s="46"/>
+      <c r="G145" s="49"/>
+      <c r="H145" s="50"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="38">
@@ -5151,8 +5154,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G146" s="43"/>
-      <c r="H146" s="46"/>
+      <c r="G146" s="49"/>
+      <c r="H146" s="50"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="38">
@@ -5174,8 +5177,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G147" s="43"/>
-      <c r="H147" s="46"/>
+      <c r="G147" s="49"/>
+      <c r="H147" s="50"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="38">
@@ -5197,8 +5200,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G148" s="43"/>
-      <c r="H148" s="46"/>
+      <c r="G148" s="49"/>
+      <c r="H148" s="50"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="38">
@@ -5220,8 +5223,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G149" s="43"/>
-      <c r="H149" s="46"/>
+      <c r="G149" s="49"/>
+      <c r="H149" s="50"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="38">
@@ -5243,8 +5246,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G150" s="43"/>
-      <c r="H150" s="46"/>
+      <c r="G150" s="49"/>
+      <c r="H150" s="50"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="38">
@@ -5266,8 +5269,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G151" s="43"/>
-      <c r="H151" s="46"/>
+      <c r="G151" s="49"/>
+      <c r="H151" s="50"/>
     </row>
     <row r="152" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A152" s="38">
@@ -5289,8 +5292,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G152" s="43"/>
-      <c r="H152" s="46"/>
+      <c r="G152" s="49"/>
+      <c r="H152" s="50"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="38">
@@ -5312,8 +5315,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G153" s="43"/>
-      <c r="H153" s="46"/>
+      <c r="G153" s="49"/>
+      <c r="H153" s="50"/>
     </row>
     <row r="154" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A154" s="38">
@@ -5335,8 +5338,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G154" s="43"/>
-      <c r="H154" s="46"/>
+      <c r="G154" s="49"/>
+      <c r="H154" s="50"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="38">
@@ -5358,8 +5361,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G155" s="43"/>
-      <c r="H155" s="46"/>
+      <c r="G155" s="49"/>
+      <c r="H155" s="50"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="38">
@@ -5381,8 +5384,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G156" s="43"/>
-      <c r="H156" s="46"/>
+      <c r="G156" s="49"/>
+      <c r="H156" s="50"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="38">
@@ -5404,8 +5407,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G157" s="43"/>
-      <c r="H157" s="46"/>
+      <c r="G157" s="49"/>
+      <c r="H157" s="50"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="38">
@@ -5427,8 +5430,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G158" s="43"/>
-      <c r="H158" s="46"/>
+      <c r="G158" s="49"/>
+      <c r="H158" s="50"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="38">
@@ -5450,8 +5453,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G159" s="43"/>
-      <c r="H159" s="46"/>
+      <c r="G159" s="49"/>
+      <c r="H159" s="50"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="38">
@@ -5473,8 +5476,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G160" s="43"/>
-      <c r="H160" s="46"/>
+      <c r="G160" s="49"/>
+      <c r="H160" s="50"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="38">
@@ -5496,8 +5499,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G161" s="43"/>
-      <c r="H161" s="46"/>
+      <c r="G161" s="49"/>
+      <c r="H161" s="50"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="38">
@@ -5519,8 +5522,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G162" s="43"/>
-      <c r="H162" s="46"/>
+      <c r="G162" s="49"/>
+      <c r="H162" s="50"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="38">
@@ -5542,8 +5545,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G163" s="43"/>
-      <c r="H163" s="46"/>
+      <c r="G163" s="49"/>
+      <c r="H163" s="50"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="38">
@@ -5565,8 +5568,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G164" s="43"/>
-      <c r="H164" s="46"/>
+      <c r="G164" s="49"/>
+      <c r="H164" s="50"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="38">
@@ -5588,8 +5591,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G165" s="43"/>
-      <c r="H165" s="46"/>
+      <c r="G165" s="49"/>
+      <c r="H165" s="50"/>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="38">
@@ -5611,8 +5614,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G166" s="43"/>
-      <c r="H166" s="46"/>
+      <c r="G166" s="49"/>
+      <c r="H166" s="50"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="38">
@@ -5634,8 +5637,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G167" s="43"/>
-      <c r="H167" s="46"/>
+      <c r="G167" s="49"/>
+      <c r="H167" s="50"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="38">
@@ -5657,8 +5660,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G168" s="43"/>
-      <c r="H168" s="46"/>
+      <c r="G168" s="49"/>
+      <c r="H168" s="50"/>
     </row>
     <row r="169" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A169" s="38">
@@ -5680,8 +5683,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G169" s="43"/>
-      <c r="H169" s="46"/>
+      <c r="G169" s="49"/>
+      <c r="H169" s="50"/>
     </row>
     <row r="170" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A170" s="38">
@@ -5703,8 +5706,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G170" s="43"/>
-      <c r="H170" s="46"/>
+      <c r="G170" s="49"/>
+      <c r="H170" s="50"/>
     </row>
     <row r="171" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A171" s="38">
@@ -5726,8 +5729,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G171" s="43"/>
-      <c r="H171" s="46"/>
+      <c r="G171" s="49"/>
+      <c r="H171" s="50"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="38">
@@ -5749,8 +5752,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G172" s="43"/>
-      <c r="H172" s="46"/>
+      <c r="G172" s="49"/>
+      <c r="H172" s="50"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="38">
@@ -5772,8 +5775,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G173" s="43"/>
-      <c r="H173" s="46"/>
+      <c r="G173" s="49"/>
+      <c r="H173" s="50"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="38">
@@ -5795,8 +5798,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G174" s="43"/>
-      <c r="H174" s="46"/>
+      <c r="G174" s="49"/>
+      <c r="H174" s="50"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="38">
@@ -5818,8 +5821,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G175" s="43"/>
-      <c r="H175" s="46"/>
+      <c r="G175" s="49"/>
+      <c r="H175" s="50"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="38">
@@ -5841,8 +5844,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G176" s="43"/>
-      <c r="H176" s="46"/>
+      <c r="G176" s="49"/>
+      <c r="H176" s="50"/>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="38">
@@ -5864,8 +5867,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G177" s="43"/>
-      <c r="H177" s="46"/>
+      <c r="G177" s="49"/>
+      <c r="H177" s="50"/>
     </row>
     <row r="178" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
       <c r="A178" s="38">
@@ -5874,7 +5877,7 @@
       <c r="B178" s="23">
         <v>5</v>
       </c>
-      <c r="C178" s="52" t="s">
+      <c r="C178" s="39" t="s">
         <v>234</v>
       </c>
       <c r="D178" s="10" t="s">
@@ -5887,20 +5890,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G178" s="43"/>
-      <c r="H178" s="46"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G178" s="49"/>
+      <c r="H178" s="50"/>
+    </row>
+    <row r="179" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A179" s="38">
         <v>177</v>
       </c>
       <c r="B179" s="23">
         <v>5</v>
       </c>
-      <c r="E179" s="18"/>
-      <c r="F179" s="18" t="str">
+      <c r="C179" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D179" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="E179" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F179" s="18">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="H179" s="22"/>
     </row>
@@ -9348,17 +9359,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="G3:G7"/>
-    <mergeCell ref="G8:G32"/>
-    <mergeCell ref="H8:H32"/>
     <mergeCell ref="G33:G53"/>
     <mergeCell ref="H33:H53"/>
     <mergeCell ref="G54:G122"/>
     <mergeCell ref="H54:H122"/>
     <mergeCell ref="G123:G178"/>
     <mergeCell ref="H123:H178"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="G8:G32"/>
+    <mergeCell ref="H8:H32"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2 H33 H54 C138 C144 C161 C167 C169 H192:H1048576 H123">
     <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Stop current Development">
@@ -9401,8 +9412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B167" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176:D177"/>
+    <sheetView tabSelected="1" topLeftCell="B176" workbookViewId="0">
+      <selection activeCell="F176" sqref="F176:H178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -9419,16 +9430,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -14265,7 +14276,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
       <c r="A177" s="9"/>
       <c r="B177" s="9">
         <f>'Bug Metrics'!$B182</f>
@@ -14279,23 +14290,45 @@
         <f>'Bug Metrics'!$D178</f>
         <v>Information about round number, status and student edollar balance is repeated on home page</v>
       </c>
-      <c r="E177" s="11"/>
-      <c r="F177" s="14"/>
-      <c r="G177" s="14"/>
-      <c r="H177" s="16"/>
-    </row>
-    <row r="178" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
+      <c r="E177" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F177" s="14">
+        <v>43786</v>
+      </c>
+      <c r="G177" s="14">
+        <v>43786</v>
+      </c>
+      <c r="H177" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="29.2" x14ac:dyDescent="0.35">
       <c r="A178" s="9"/>
       <c r="B178" s="9">
         <f>'Bug Metrics'!$B183</f>
         <v>5</v>
       </c>
-      <c r="C178" s="9"/>
-      <c r="D178" s="10"/>
-      <c r="E178" s="11"/>
-      <c r="F178" s="14"/>
-      <c r="G178" s="14"/>
-      <c r="H178" s="16"/>
+      <c r="C178" s="9" t="str">
+        <f>'Bug Metrics'!$C179</f>
+        <v>Dump</v>
+      </c>
+      <c r="D178" s="10" t="str">
+        <f>'Bug Metrics'!$D179</f>
+        <v>Test case 185-dump - section-student is populated with ALL successful bids across round 1 and round 2, should only should previous round</v>
+      </c>
+      <c r="E178" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F178" s="14">
+        <v>43786</v>
+      </c>
+      <c r="G178" s="14">
+        <v>43786</v>
+      </c>
+      <c r="H178" s="16" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="179" spans="1:8" ht="14.6" x14ac:dyDescent="0.35">
       <c r="A179" s="9"/>
@@ -22648,49 +22681,49 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E32 E34:E200">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E32 E34:E200">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E32 E34:E200">
-    <cfRule type="containsBlanks" dxfId="8" priority="11">
+    <cfRule type="containsBlanks" dxfId="0" priority="11">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="containsBlanks" dxfId="5" priority="8">
+    <cfRule type="containsBlanks" dxfId="8" priority="8">
       <formula>LEN(TRIM(E33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>